<commit_message>
i460--Greed mode bug fix
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_12_Avant_GX.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_12_Avant_GX.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conversion\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709C3E94-1C8A-40D4-A855-17262A1CD9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="pSvbrBtM5D7J1tTbaFvNMFAx+gsFF1+zjWgivCK1irAkzVtGcdIaviGYDMewqTuAFCctlIpswoSn4Z8ezPPc6w==" workbookSaltValue="fuR2EkRIGc7n0eTkIKsWWA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
@@ -27,10 +28,10 @@
   </definedNames>
   <calcPr calcId="122211"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" mergeInterval="0" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Jeffrey Ye - Personal View" guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="3"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -2280,9 +2281,6 @@
     <t>ITR5_GX/51_MPP/01_impl/101_MPPCIEX8_impl</t>
   </si>
   <si>
-    <t>ITR5_GX/51_MPP/01_impl/221_MPPHYX4_impl</t>
-  </si>
-  <si>
     <t>ITR5_GX/51_MPP/03_sim/101_MPPCIEX8_sim</t>
   </si>
   <si>
@@ -2410,12 +2408,15 @@
   </si>
   <si>
     <t xml:space="preserve">cmd = python DEV/bin/run_radiant.py  --run-map-trce --run-par-trce </t>
+  </si>
+  <si>
+    <t>ITR5_GX/51_MPP/01_impl/201_MPPHYX4_impl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00_ "/>
     <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
@@ -3506,7 +3507,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -3514,13 +3515,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47">
@@ -3580,7 +3581,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
@@ -3616,22 +3617,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="47" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="41" xfId="47" applyBorder="1" applyAlignment="1">
@@ -3661,22 +3653,16 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="49" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="15" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="16" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="18" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3691,25 +3677,19 @@
     <xf numFmtId="165" fontId="21" fillId="0" borderId="24" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="42" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="43" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="44" xfId="47" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="21" fillId="0" borderId="21" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="21" fillId="0" borderId="22" xfId="47" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="7" borderId="27" xfId="13" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3724,31 +3704,64 @@
     <xf numFmtId="49" fontId="12" fillId="7" borderId="7" xfId="13" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3760,13 +3773,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="47" applyBorder="1" applyAlignment="1">
@@ -3786,44 +3793,17 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="48" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="48" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="37" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="38" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" xfId="47" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -3860,19 +3840,19 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink 2" xfId="49"/>
+    <cellStyle name="Hyperlink 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="41"/>
-    <cellStyle name="Normal 2 2" xfId="47"/>
-    <cellStyle name="Normal 3" xfId="44"/>
-    <cellStyle name="Normal 4" xfId="45"/>
-    <cellStyle name="Normal 5" xfId="46"/>
-    <cellStyle name="Normal 6" xfId="43"/>
-    <cellStyle name="Normal 6 2" xfId="48"/>
-    <cellStyle name="Note 2" xfId="42"/>
+    <cellStyle name="Normal 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 2 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 4" xfId="45" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 5" xfId="46" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 6" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 6 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Note 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
@@ -6488,6 +6468,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -6523,6 +6520,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6698,14 +6712,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="2" customWidth="1"/>
@@ -6733,7 +6747,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -6754,7 +6768,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -6762,7 +6776,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6930,23 +6944,23 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
+      <selection activeCell="C52" sqref="C52"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" topLeftCell="A2">
-      <selection activeCell="C52" sqref="C52"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -6958,7 +6972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE202"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -6966,76 +6980,76 @@
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="A2" sqref="A2"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E206" sqref="E206"/>
+      <selection pane="bottomRight" activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="60.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="60.109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" style="2" customWidth="1"/>
     <col min="7" max="7" width="24" style="2" customWidth="1"/>
     <col min="8" max="8" width="37" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="38" style="2" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" style="2" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="30.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="17.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" style="2" customWidth="1"/>
     <col min="18" max="18" width="13" style="2" customWidth="1"/>
-    <col min="19" max="20" width="9.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="9.42578125" style="2" customWidth="1"/>
+    <col min="19" max="20" width="9.6640625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="9.44140625" style="2" customWidth="1"/>
     <col min="22" max="22" width="11" style="2" customWidth="1"/>
-    <col min="23" max="23" width="11.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" style="2" customWidth="1"/>
     <col min="24" max="29" width="9" style="2"/>
-    <col min="30" max="30" width="10.140625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="10.109375" style="2" customWidth="1"/>
     <col min="31" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:31" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+      <c r="A1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="71"/>
-      <c r="X1" s="72" t="s">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
+      <c r="Q1" s="63"/>
+      <c r="R1" s="63"/>
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="63"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="72"/>
-    </row>
-    <row r="2" spans="1:31" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+    </row>
+    <row r="2" spans="1:31" s="3" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -7130,7 +7144,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15.75" thickTop="1">
+    <row r="3" spans="1:31" ht="15" thickTop="1">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -11424,7 +11438,7 @@
         <v>735</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>737</v>
+        <v>780</v>
       </c>
       <c r="S166" s="2" t="s">
         <v>301</v>
@@ -11441,7 +11455,7 @@
         <v>735</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="S167" s="2" t="s">
         <v>301</v>
@@ -11458,7 +11472,7 @@
         <v>735</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="S168" s="2" t="s">
         <v>301</v>
@@ -11475,10 +11489,10 @@
         <v>518</v>
       </c>
       <c r="E169" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="H169" s="2" t="s">
         <v>740</v>
-      </c>
-      <c r="H169" s="2" t="s">
-        <v>741</v>
       </c>
       <c r="S169" s="2" t="s">
         <v>301</v>
@@ -11495,10 +11509,10 @@
         <v>518</v>
       </c>
       <c r="E170" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="H170" s="2" t="s">
         <v>742</v>
-      </c>
-      <c r="H170" s="2" t="s">
-        <v>743</v>
       </c>
       <c r="S170" s="2" t="s">
         <v>301</v>
@@ -11515,10 +11529,10 @@
         <v>518</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="H171" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="S171" s="2" t="s">
         <v>301</v>
@@ -11535,10 +11549,10 @@
         <v>518</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H172" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="S172" s="2" t="s">
         <v>301</v>
@@ -11552,10 +11566,10 @@
     </row>
     <row r="173" spans="1:31">
       <c r="D173" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="E173" s="2" t="s">
         <v>746</v>
-      </c>
-      <c r="E173" s="2" t="s">
-        <v>747</v>
       </c>
       <c r="S173" s="2" t="s">
         <v>301</v>
@@ -11569,10 +11583,10 @@
     </row>
     <row r="174" spans="1:31">
       <c r="D174" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="S174" s="2" t="s">
         <v>301</v>
@@ -11586,10 +11600,10 @@
     </row>
     <row r="175" spans="1:31">
       <c r="D175" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="S175" s="2" t="s">
         <v>301</v>
@@ -11603,10 +11617,10 @@
     </row>
     <row r="176" spans="1:31">
       <c r="D176" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="S176" s="2" t="s">
         <v>301</v>
@@ -11620,10 +11634,10 @@
     </row>
     <row r="177" spans="4:31">
       <c r="D177" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="S177" s="2" t="s">
         <v>301</v>
@@ -11637,10 +11651,10 @@
     </row>
     <row r="178" spans="4:31">
       <c r="D178" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="S178" s="2" t="s">
         <v>301</v>
@@ -11654,10 +11668,10 @@
     </row>
     <row r="179" spans="4:31">
       <c r="D179" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="S179" s="2" t="s">
         <v>301</v>
@@ -11671,10 +11685,10 @@
     </row>
     <row r="180" spans="4:31">
       <c r="D180" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="S180" s="2" t="s">
         <v>301</v>
@@ -11688,10 +11702,10 @@
     </row>
     <row r="181" spans="4:31">
       <c r="D181" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="S181" s="2" t="s">
         <v>301</v>
@@ -11705,10 +11719,10 @@
     </row>
     <row r="182" spans="4:31">
       <c r="D182" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="S182" s="2" t="s">
         <v>301</v>
@@ -11722,10 +11736,10 @@
     </row>
     <row r="183" spans="4:31">
       <c r="D183" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="S183" s="2" t="s">
         <v>301</v>
@@ -11739,10 +11753,10 @@
     </row>
     <row r="184" spans="4:31">
       <c r="D184" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="S184" s="2" t="s">
         <v>301</v>
@@ -11756,10 +11770,10 @@
     </row>
     <row r="185" spans="4:31">
       <c r="D185" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="S185" s="2" t="s">
         <v>301</v>
@@ -11773,10 +11787,10 @@
     </row>
     <row r="186" spans="4:31">
       <c r="D186" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="S186" s="2" t="s">
         <v>301</v>
@@ -11790,10 +11804,10 @@
     </row>
     <row r="187" spans="4:31">
       <c r="D187" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="S187" s="2" t="s">
         <v>301</v>
@@ -11807,10 +11821,10 @@
     </row>
     <row r="188" spans="4:31">
       <c r="D188" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E188" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="S188" s="2" t="s">
         <v>301</v>
@@ -11824,10 +11838,10 @@
     </row>
     <row r="189" spans="4:31">
       <c r="D189" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="S189" s="2" t="s">
         <v>301</v>
@@ -11841,10 +11855,10 @@
     </row>
     <row r="190" spans="4:31">
       <c r="D190" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E190" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="S190" s="2" t="s">
         <v>301</v>
@@ -11858,10 +11872,10 @@
     </row>
     <row r="191" spans="4:31">
       <c r="D191" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E191" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="S191" s="2" t="s">
         <v>301</v>
@@ -11875,10 +11889,10 @@
     </row>
     <row r="192" spans="4:31">
       <c r="D192" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="S192" s="2" t="s">
         <v>301</v>
@@ -11892,10 +11906,10 @@
     </row>
     <row r="193" spans="4:31">
       <c r="D193" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="S193" s="2" t="s">
         <v>301</v>
@@ -11909,10 +11923,10 @@
     </row>
     <row r="194" spans="4:31">
       <c r="D194" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E194" s="2" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="S194" s="2" t="s">
         <v>301</v>
@@ -11926,10 +11940,10 @@
     </row>
     <row r="195" spans="4:31">
       <c r="D195" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="S195" s="2" t="s">
         <v>301</v>
@@ -11943,10 +11957,10 @@
     </row>
     <row r="196" spans="4:31">
       <c r="D196" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="S196" s="2" t="s">
         <v>301</v>
@@ -11960,10 +11974,10 @@
     </row>
     <row r="197" spans="4:31">
       <c r="D197" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E197" s="2" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="S197" s="2" t="s">
         <v>301</v>
@@ -11977,10 +11991,10 @@
     </row>
     <row r="198" spans="4:31">
       <c r="D198" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E198" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="S198" s="2" t="s">
         <v>301</v>
@@ -11994,10 +12008,10 @@
     </row>
     <row r="199" spans="4:31">
       <c r="D199" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="S199" s="2" t="s">
         <v>301</v>
@@ -12011,10 +12025,10 @@
     </row>
     <row r="200" spans="4:31">
       <c r="D200" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="S200" s="2" t="s">
         <v>301</v>
@@ -12028,10 +12042,10 @@
     </row>
     <row r="201" spans="4:31">
       <c r="D201" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="E201" s="2" t="s">
         <v>775</v>
-      </c>
-      <c r="E201" s="2" t="s">
-        <v>776</v>
       </c>
       <c r="S201" s="2" t="s">
         <v>301</v>
@@ -12045,10 +12059,10 @@
     </row>
     <row r="202" spans="4:31">
       <c r="D202" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="S202" s="2" t="s">
         <v>301</v>
@@ -12062,14 +12076,14 @@
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="oSh3vRnxVqjddGqXIe7WCBtY0UIhfw+5hx9hFmwK+zOVJn30i2qdL6F35lxIbLPoaaesJXtjEAYmG4HcQFEykg==" saltValue="88e6IcLciP+0JP9xgq1/0Q==" spinCount="100000" sheet="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A2:AE162"/>
+  <autoFilter ref="A2:AE162" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="2">
     <mergeCell ref="A1:W1"/>
     <mergeCell ref="X1:AE1"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1 M1:AB1 G1:H1 C1:E1 A1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1 M1:AB1 G1:H1 C1:E1 A1" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -12078,49 +12092,49 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>description!$F$120:$K$120</xm:f>
           </x14:formula1>
           <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>description!$F$117:$H$117</xm:f>
           </x14:formula1>
           <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>description!$E$113:$F$113</xm:f>
           </x14:formula1>
           <xm:sqref>B1:B1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>description!$F$123:$H$123</xm:f>
           </x14:formula1>
           <xm:sqref>L1:L1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000005000000}">
           <x14:formula1>
             <xm:f>description!$F$121:$K$121</xm:f>
           </x14:formula1>
           <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000006000000}">
           <x14:formula1>
             <xm:f>description!$F$122:$H$122</xm:f>
           </x14:formula1>
           <xm:sqref>K1:K1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000007000000}">
           <x14:formula1>
             <xm:f>description!$F$142:$H$142</xm:f>
           </x14:formula1>
           <xm:sqref>AD1:AD1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000008000000}">
           <x14:formula1>
             <xm:f>description!$F$141:$H$141</xm:f>
           </x14:formula1>
@@ -12133,25 +12147,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N243"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C210" sqref="C210:E210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="19" style="6" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="15" style="6" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.88671875" style="6" customWidth="1"/>
     <col min="6" max="6" width="32" style="6" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="28.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="6" customWidth="1"/>
+    <col min="7" max="7" width="31.6640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" style="6" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="6" customWidth="1"/>
     <col min="11" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
@@ -12174,7 +12188,7 @@
     <row r="107" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="108" spans="1:14" ht="12.75" customHeight="1"/>
     <row r="109" spans="1:14" ht="12.75" customHeight="1"/>
-    <row r="110" spans="1:14" ht="15.75" thickBot="1">
+    <row r="110" spans="1:14" ht="15" thickBot="1">
       <c r="A110" s="6" t="s">
         <v>81</v>
       </c>
@@ -12182,7 +12196,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="15.75" thickBot="1">
+    <row r="111" spans="1:14" ht="15" thickBot="1">
       <c r="A111" s="9" t="s">
         <v>83</v>
       </c>
@@ -12198,17 +12212,17 @@
       <c r="E111" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F111" s="75" t="s">
+      <c r="F111" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="G111" s="76"/>
-      <c r="H111" s="76"/>
-      <c r="I111" s="76"/>
-      <c r="J111" s="76"/>
-      <c r="K111" s="76"/>
-      <c r="L111" s="76"/>
-      <c r="M111" s="76"/>
-      <c r="N111" s="77"/>
+      <c r="G111" s="100"/>
+      <c r="H111" s="100"/>
+      <c r="I111" s="100"/>
+      <c r="J111" s="100"/>
+      <c r="K111" s="100"/>
+      <c r="L111" s="100"/>
+      <c r="M111" s="100"/>
+      <c r="N111" s="101"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="11" t="s">
@@ -13036,7 +13050,7 @@
       <c r="M142" s="18"/>
       <c r="N142" s="19"/>
     </row>
-    <row r="143" spans="1:14" ht="15.75" thickBot="1">
+    <row r="143" spans="1:14" ht="15" thickBot="1">
       <c r="A143" s="20" t="s">
         <v>122</v>
       </c>
@@ -13060,7 +13074,7 @@
       <c r="M143" s="21"/>
       <c r="N143" s="22"/>
     </row>
-    <row r="146" spans="1:8" ht="15.75" thickBot="1">
+    <row r="146" spans="1:8" ht="15" thickBot="1">
       <c r="A146" s="6" t="s">
         <v>123</v>
       </c>
@@ -13098,7 +13112,7 @@
       <c r="A148" s="26">
         <v>1</v>
       </c>
-      <c r="B148" s="78" t="s">
+      <c r="B148" s="84" t="s">
         <v>3</v>
       </c>
       <c r="C148" s="27" t="s">
@@ -13124,7 +13138,7 @@
       <c r="A149" s="26">
         <v>2</v>
       </c>
-      <c r="B149" s="79"/>
+      <c r="B149" s="85"/>
       <c r="C149" s="28" t="s">
         <v>136</v>
       </c>
@@ -13146,7 +13160,7 @@
       <c r="A150" s="26">
         <v>3</v>
       </c>
-      <c r="B150" s="79"/>
+      <c r="B150" s="85"/>
       <c r="C150" s="28" t="s">
         <v>9</v>
       </c>
@@ -13166,7 +13180,7 @@
       <c r="A151" s="26">
         <v>4</v>
       </c>
-      <c r="B151" s="79"/>
+      <c r="B151" s="85"/>
       <c r="C151" s="28" t="s">
         <v>138</v>
       </c>
@@ -13190,7 +13204,7 @@
       <c r="A152" s="26">
         <v>5</v>
       </c>
-      <c r="B152" s="79"/>
+      <c r="B152" s="85"/>
       <c r="C152" s="27" t="s">
         <v>140</v>
       </c>
@@ -13214,7 +13228,7 @@
       <c r="A153" s="26">
         <v>6</v>
       </c>
-      <c r="B153" s="79"/>
+      <c r="B153" s="85"/>
       <c r="C153" s="27" t="s">
         <v>144</v>
       </c>
@@ -13238,7 +13252,7 @@
       <c r="A154" s="26">
         <v>7</v>
       </c>
-      <c r="B154" s="79"/>
+      <c r="B154" s="85"/>
       <c r="C154" s="28" t="s">
         <v>147</v>
       </c>
@@ -13260,7 +13274,7 @@
       <c r="A155" s="26">
         <v>8</v>
       </c>
-      <c r="B155" s="79"/>
+      <c r="B155" s="85"/>
       <c r="C155" s="27" t="s">
         <v>148</v>
       </c>
@@ -13284,7 +13298,7 @@
       <c r="A156" s="26">
         <v>9</v>
       </c>
-      <c r="B156" s="79"/>
+      <c r="B156" s="85"/>
       <c r="C156" s="27" t="s">
         <v>149</v>
       </c>
@@ -13308,7 +13322,7 @@
       <c r="A157" s="26">
         <v>10</v>
       </c>
-      <c r="B157" s="79"/>
+      <c r="B157" s="85"/>
       <c r="C157" s="28" t="s">
         <v>150</v>
       </c>
@@ -13332,8 +13346,8 @@
       <c r="A158" s="26">
         <v>11</v>
       </c>
-      <c r="B158" s="79"/>
-      <c r="C158" s="68" t="s">
+      <c r="B158" s="85"/>
+      <c r="C158" s="27" t="s">
         <v>151</v>
       </c>
       <c r="D158" s="28" t="s">
@@ -13342,7 +13356,7 @@
       <c r="E158" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="F158" s="68" t="s">
+      <c r="F158" s="27" t="s">
         <v>253</v>
       </c>
       <c r="G158" s="28" t="s">
@@ -13356,7 +13370,7 @@
       <c r="A159" s="26">
         <v>12</v>
       </c>
-      <c r="B159" s="79"/>
+      <c r="B159" s="85"/>
       <c r="C159" s="28" t="s">
         <v>153</v>
       </c>
@@ -13378,7 +13392,7 @@
       <c r="A160" s="26">
         <v>13</v>
       </c>
-      <c r="B160" s="80"/>
+      <c r="B160" s="79"/>
       <c r="C160" s="28" t="s">
         <v>56</v>
       </c>
@@ -13402,7 +13416,7 @@
       <c r="A161" s="26">
         <v>14</v>
       </c>
-      <c r="B161" s="73" t="s">
+      <c r="B161" s="75" t="s">
         <v>4</v>
       </c>
       <c r="C161" s="28" t="s">
@@ -13452,7 +13466,7 @@
       <c r="A163" s="26">
         <v>16</v>
       </c>
-      <c r="B163" s="78" t="s">
+      <c r="B163" s="84" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="28" t="s">
@@ -13476,7 +13490,7 @@
       <c r="A164" s="26">
         <v>17</v>
       </c>
-      <c r="B164" s="81"/>
+      <c r="B164" s="102"/>
       <c r="C164" s="27" t="s">
         <v>165</v>
       </c>
@@ -13498,7 +13512,7 @@
       <c r="A165" s="26">
         <v>18</v>
       </c>
-      <c r="B165" s="80"/>
+      <c r="B165" s="79"/>
       <c r="C165" s="27" t="s">
         <v>167</v>
       </c>
@@ -13518,7 +13532,7 @@
       <c r="A166" s="26">
         <v>19</v>
       </c>
-      <c r="B166" s="73" t="s">
+      <c r="B166" s="75" t="s">
         <v>6</v>
       </c>
       <c r="C166" s="28" t="s">
@@ -13678,11 +13692,11 @@
       </c>
       <c r="H173" s="16"/>
     </row>
-    <row r="174" spans="1:8" ht="90">
+    <row r="174" spans="1:8" ht="86.4">
       <c r="A174" s="26">
         <v>27</v>
       </c>
-      <c r="B174" s="73" t="s">
+      <c r="B174" s="75" t="s">
         <v>7</v>
       </c>
       <c r="C174" s="28" t="s">
@@ -13750,7 +13764,7 @@
       <c r="A177" s="26">
         <v>30</v>
       </c>
-      <c r="B177" s="78" t="s">
+      <c r="B177" s="84" t="s">
         <v>8</v>
       </c>
       <c r="C177" s="28" t="s">
@@ -13772,11 +13786,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="15.75" thickBot="1">
+    <row r="178" spans="1:8" ht="15" thickBot="1">
       <c r="A178" s="31">
         <v>31</v>
       </c>
-      <c r="B178" s="79"/>
+      <c r="B178" s="85"/>
       <c r="C178" s="32" t="s">
         <v>189</v>
       </c>
@@ -13800,7 +13814,7 @@
       <c r="A179" s="23">
         <v>32</v>
       </c>
-      <c r="B179" s="82" t="s">
+      <c r="B179" s="86" t="s">
         <v>191</v>
       </c>
       <c r="C179" s="33" t="s">
@@ -13824,7 +13838,7 @@
       <c r="A180" s="26">
         <v>33</v>
       </c>
-      <c r="B180" s="83"/>
+      <c r="B180" s="87"/>
       <c r="C180" s="27" t="s">
         <v>195</v>
       </c>
@@ -13846,7 +13860,7 @@
       <c r="A181" s="26">
         <v>34</v>
       </c>
-      <c r="B181" s="84"/>
+      <c r="B181" s="88"/>
       <c r="C181" s="34" t="s">
         <v>198</v>
       </c>
@@ -13868,7 +13882,7 @@
       <c r="A182" s="31">
         <v>35</v>
       </c>
-      <c r="B182" s="84"/>
+      <c r="B182" s="88"/>
       <c r="C182" s="34" t="s">
         <v>199</v>
       </c>
@@ -13890,17 +13904,17 @@
       <c r="A183" s="31">
         <v>36</v>
       </c>
-      <c r="B183" s="84"/>
+      <c r="B183" s="88"/>
       <c r="C183" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="D183" s="42" t="s">
+      <c r="D183" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E183" s="42" t="s">
+      <c r="E183" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="F183" s="42"/>
+      <c r="F183" s="32"/>
       <c r="G183" s="34" t="s">
         <v>260</v>
       </c>
@@ -13910,15 +13924,15 @@
       <c r="A184" s="31">
         <v>37</v>
       </c>
-      <c r="B184" s="84"/>
+      <c r="B184" s="88"/>
       <c r="C184" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="D184" s="42" t="s">
+      <c r="D184" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E184" s="42"/>
-      <c r="F184" s="42" t="s">
+      <c r="E184" s="32"/>
+      <c r="F184" s="32" t="s">
         <v>255</v>
       </c>
       <c r="G184" s="34" t="s">
@@ -13928,11 +13942,11 @@
         <v>257</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="15.75" thickBot="1">
+    <row r="185" spans="1:8" ht="15" thickBot="1">
       <c r="A185" s="35">
         <v>38</v>
       </c>
-      <c r="B185" s="85"/>
+      <c r="B185" s="83"/>
       <c r="C185" s="36" t="s">
         <v>258</v>
       </c>
@@ -13959,7 +13973,7 @@
       </c>
     </row>
     <row r="187" spans="1:8">
-      <c r="B187" s="37" t="s">
+      <c r="B187" s="6" t="s">
         <v>205</v>
       </c>
     </row>
@@ -13968,7 +13982,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="15.75" thickBot="1">
+    <row r="198" spans="1:7" ht="15" thickBot="1">
       <c r="A198" s="6" t="s">
         <v>207</v>
       </c>
@@ -13980,159 +13994,159 @@
       <c r="A199" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B199" s="38" t="s">
+      <c r="B199" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="C199" s="86" t="s">
+      <c r="C199" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="D199" s="86"/>
-      <c r="E199" s="86"/>
-      <c r="F199" s="39" t="s">
+      <c r="D199" s="89"/>
+      <c r="E199" s="89"/>
+      <c r="F199" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="G199" s="40" t="s">
+      <c r="G199" s="38" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="200" spans="1:7">
-      <c r="A200" s="87" t="s">
+      <c r="A200" s="72" t="s">
         <v>212</v>
       </c>
       <c r="B200" s="74" t="s">
         <v>213</v>
       </c>
-      <c r="C200" s="89" t="s">
+      <c r="C200" s="91" t="s">
         <v>57</v>
       </c>
-      <c r="D200" s="90"/>
-      <c r="E200" s="90"/>
+      <c r="D200" s="92"/>
+      <c r="E200" s="92"/>
       <c r="F200" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G200" s="41" t="s">
+      <c r="G200" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="87"/>
-      <c r="B201" s="88"/>
-      <c r="C201" s="91" t="s">
+      <c r="A201" s="72"/>
+      <c r="B201" s="90"/>
+      <c r="C201" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="D201" s="92"/>
-      <c r="E201" s="92"/>
+      <c r="D201" s="94"/>
+      <c r="E201" s="94"/>
       <c r="F201" s="32" t="s">
         <v>215</v>
       </c>
-      <c r="G201" s="43" t="s">
+      <c r="G201" s="40" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="202" spans="1:7">
-      <c r="A202" s="87"/>
+      <c r="A202" s="72"/>
       <c r="B202" s="74" t="s">
         <v>216</v>
       </c>
-      <c r="C202" s="93" t="s">
+      <c r="C202" s="95" t="s">
         <v>217</v>
       </c>
-      <c r="D202" s="93"/>
-      <c r="E202" s="93"/>
+      <c r="D202" s="95"/>
+      <c r="E202" s="95"/>
       <c r="F202" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G202" s="41" t="s">
+      <c r="G202" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="203" spans="1:7">
-      <c r="A203" s="87"/>
+      <c r="A203" s="72"/>
       <c r="B203" s="74"/>
-      <c r="C203" s="91" t="s">
+      <c r="C203" s="93" t="s">
         <v>217</v>
       </c>
-      <c r="D203" s="91"/>
-      <c r="E203" s="91"/>
+      <c r="D203" s="93"/>
+      <c r="E203" s="93"/>
       <c r="F203" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G203" s="41" t="s">
+      <c r="G203" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="87"/>
-      <c r="B204" s="88" t="s">
+      <c r="A204" s="72"/>
+      <c r="B204" s="90" t="s">
         <v>218</v>
       </c>
-      <c r="C204" s="94" t="s">
+      <c r="C204" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="D204" s="95"/>
-      <c r="E204" s="96"/>
+      <c r="D204" s="97"/>
+      <c r="E204" s="98"/>
       <c r="F204" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G204" s="41" t="s">
+      <c r="G204" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="87"/>
-      <c r="B205" s="80"/>
-      <c r="C205" s="94" t="s">
+      <c r="A205" s="72"/>
+      <c r="B205" s="79"/>
+      <c r="C205" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="D205" s="95"/>
-      <c r="E205" s="96"/>
+      <c r="D205" s="97"/>
+      <c r="E205" s="98"/>
       <c r="F205" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G205" s="41" t="s">
+      <c r="G205" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="87"/>
+      <c r="A206" s="72"/>
       <c r="B206" s="74" t="s">
         <v>219</v>
       </c>
-      <c r="C206" s="93" t="s">
+      <c r="C206" s="95" t="s">
         <v>220</v>
       </c>
-      <c r="D206" s="93"/>
-      <c r="E206" s="93"/>
+      <c r="D206" s="95"/>
+      <c r="E206" s="95"/>
       <c r="F206" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G206" s="41" t="s">
+      <c r="G206" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="87"/>
+      <c r="A207" s="72"/>
       <c r="B207" s="74"/>
-      <c r="C207" s="93" t="s">
+      <c r="C207" s="95" t="s">
         <v>220</v>
       </c>
-      <c r="D207" s="93"/>
-      <c r="E207" s="93"/>
+      <c r="D207" s="95"/>
+      <c r="E207" s="95"/>
       <c r="F207" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G207" s="41" t="s">
+      <c r="G207" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="87" t="s">
+      <c r="A208" s="72" t="s">
         <v>221</v>
       </c>
       <c r="B208" s="74" t="s">
         <v>222</v>
       </c>
-      <c r="C208" s="73" t="s">
+      <c r="C208" s="75" t="s">
         <v>45</v>
       </c>
       <c r="D208" s="74"/>
@@ -14140,12 +14154,12 @@
       <c r="F208" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G208" s="41" t="s">
+      <c r="G208" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="87"/>
+      <c r="A209" s="72"/>
       <c r="B209" s="74"/>
       <c r="C209" s="74" t="s">
         <v>46</v>
@@ -14155,16 +14169,16 @@
       <c r="F209" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G209" s="41" t="s">
+      <c r="G209" s="39" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="87"/>
+      <c r="A210" s="72"/>
       <c r="B210" s="74" t="s">
         <v>224</v>
       </c>
-      <c r="C210" s="73" t="s">
+      <c r="C210" s="75" t="s">
         <v>47</v>
       </c>
       <c r="D210" s="74"/>
@@ -14172,12 +14186,12 @@
       <c r="F210" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G210" s="41" t="s">
+      <c r="G210" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="87"/>
+      <c r="A211" s="72"/>
       <c r="B211" s="74"/>
       <c r="C211" s="74" t="s">
         <v>48</v>
@@ -14187,18 +14201,18 @@
       <c r="F211" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G211" s="41" t="s">
+      <c r="G211" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="87" t="s">
+      <c r="A212" s="72" t="s">
         <v>225</v>
       </c>
       <c r="B212" s="74" t="s">
         <v>226</v>
       </c>
-      <c r="C212" s="73" t="s">
+      <c r="C212" s="75" t="s">
         <v>49</v>
       </c>
       <c r="D212" s="74"/>
@@ -14206,12 +14220,12 @@
       <c r="F212" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G212" s="41" t="s">
+      <c r="G212" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="87"/>
+      <c r="A213" s="72"/>
       <c r="B213" s="74"/>
       <c r="C213" s="74" t="s">
         <v>50</v>
@@ -14221,16 +14235,16 @@
       <c r="F213" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="G213" s="41" t="s">
+      <c r="G213" s="39" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="87"/>
+      <c r="A214" s="72"/>
       <c r="B214" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="C214" s="73" t="s">
+      <c r="C214" s="75" t="s">
         <v>228</v>
       </c>
       <c r="D214" s="74"/>
@@ -14238,22 +14252,22 @@
       <c r="F214" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="G214" s="41" t="s">
+      <c r="G214" s="39" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A215" s="98"/>
-      <c r="B215" s="99"/>
-      <c r="C215" s="99" t="s">
+    <row r="215" spans="1:7" ht="15" thickBot="1">
+      <c r="A215" s="73"/>
+      <c r="B215" s="76"/>
+      <c r="C215" s="76" t="s">
         <v>229</v>
       </c>
-      <c r="D215" s="99"/>
-      <c r="E215" s="99"/>
+      <c r="D215" s="76"/>
+      <c r="E215" s="76"/>
       <c r="F215" s="36" t="s">
         <v>215</v>
       </c>
-      <c r="G215" s="44" t="s">
+      <c r="G215" s="41" t="s">
         <v>63</v>
       </c>
     </row>
@@ -14261,60 +14275,43 @@
       <c r="A216" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="C216" s="37"/>
-      <c r="D216" s="37"/>
-      <c r="E216" s="37"/>
-      <c r="F216" s="37"/>
-    </row>
-    <row r="217" spans="1:7">
-      <c r="C217" s="37"/>
-      <c r="D217" s="37"/>
-      <c r="E217" s="37"/>
-    </row>
-    <row r="218" spans="1:7">
-      <c r="C218" s="37"/>
-      <c r="D218" s="37"/>
-      <c r="E218" s="37"/>
-    </row>
-    <row r="219" spans="1:7" ht="15.75" thickBot="1">
+    </row>
+    <row r="219" spans="1:7" ht="15" thickBot="1">
       <c r="A219" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="C219" s="37"/>
-      <c r="D219" s="37"/>
-      <c r="E219" s="37"/>
-    </row>
-    <row r="220" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A220" s="45" t="s">
+    </row>
+    <row r="220" spans="1:7" ht="15" thickBot="1">
+      <c r="A220" s="42" t="s">
         <v>232</v>
       </c>
-      <c r="B220" s="100" t="s">
+      <c r="B220" s="77" t="s">
         <v>52</v>
       </c>
-      <c r="C220" s="100"/>
-      <c r="D220" s="100"/>
-      <c r="E220" s="100"/>
-      <c r="F220" s="46" t="s">
+      <c r="C220" s="77"/>
+      <c r="D220" s="77"/>
+      <c r="E220" s="77"/>
+      <c r="F220" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="G220" s="47" t="s">
+      <c r="G220" s="44" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="221" spans="1:7" ht="93" customHeight="1">
-      <c r="A221" s="48" t="s">
+      <c r="A221" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="B221" s="101" t="s">
+      <c r="B221" s="78" t="s">
         <v>236</v>
       </c>
-      <c r="C221" s="80"/>
-      <c r="D221" s="80"/>
-      <c r="E221" s="80"/>
-      <c r="F221" s="49" t="s">
+      <c r="C221" s="79"/>
+      <c r="D221" s="79"/>
+      <c r="E221" s="79"/>
+      <c r="F221" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="G221" s="50" t="s">
+      <c r="G221" s="47" t="s">
         <v>63</v>
       </c>
     </row>
@@ -14322,12 +14319,12 @@
       <c r="A222" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="B222" s="102" t="s">
+      <c r="B222" s="80" t="s">
         <v>238</v>
       </c>
-      <c r="C222" s="103"/>
-      <c r="D222" s="103"/>
-      <c r="E222" s="104"/>
+      <c r="C222" s="81"/>
+      <c r="D222" s="81"/>
+      <c r="E222" s="82"/>
       <c r="F222" s="15" t="s">
         <v>63</v>
       </c>
@@ -14339,12 +14336,12 @@
       <c r="A223" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B223" s="102" t="s">
+      <c r="B223" s="80" t="s">
         <v>239</v>
       </c>
-      <c r="C223" s="103"/>
-      <c r="D223" s="103"/>
-      <c r="E223" s="104"/>
+      <c r="C223" s="81"/>
+      <c r="D223" s="81"/>
+      <c r="E223" s="82"/>
       <c r="F223" s="18" t="s">
         <v>63</v>
       </c>
@@ -14356,12 +14353,12 @@
       <c r="A224" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="B224" s="85" t="s">
+      <c r="B224" s="83" t="s">
         <v>241</v>
       </c>
-      <c r="C224" s="99"/>
-      <c r="D224" s="99"/>
-      <c r="E224" s="99"/>
+      <c r="C224" s="76"/>
+      <c r="D224" s="76"/>
+      <c r="E224" s="76"/>
       <c r="F224" s="21" t="s">
         <v>63</v>
       </c>
@@ -14370,330 +14367,307 @@
       </c>
     </row>
     <row r="225" spans="1:7">
-      <c r="C225" s="51"/>
-    </row>
-    <row r="227" spans="1:7" ht="15.75" thickBot="1">
+      <c r="C225" s="48"/>
+    </row>
+    <row r="227" spans="1:7" ht="15" thickBot="1">
       <c r="A227" s="6" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="15.75" thickBot="1">
+    <row r="228" spans="1:7" ht="15" thickBot="1">
       <c r="A228" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="B228" s="38" t="s">
+      <c r="B228" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C228" s="52" t="s">
+      <c r="C228" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="D228" s="53" t="s">
+      <c r="D228" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E228" s="53"/>
-      <c r="F228" s="54"/>
-      <c r="G228" s="40" t="s">
+      <c r="E228" s="50"/>
+      <c r="F228" s="10"/>
+      <c r="G228" s="38" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="229" spans="1:7">
-      <c r="A229" s="55">
+      <c r="A229" s="51">
         <v>42682</v>
       </c>
-      <c r="B229" s="56">
+      <c r="B229" s="52">
         <v>1.04</v>
       </c>
       <c r="C229" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D229" s="97" t="s">
+      <c r="D229" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="E229" s="97"/>
-      <c r="F229" s="97"/>
-      <c r="G229" s="57"/>
+      <c r="E229" s="71"/>
+      <c r="F229" s="71"/>
+      <c r="G229" s="25"/>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="58">
+      <c r="A230" s="53">
         <v>42692</v>
       </c>
-      <c r="B230" s="59">
+      <c r="B230" s="54">
         <v>1.05</v>
       </c>
       <c r="C230" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D230" s="109" t="s">
+      <c r="D230" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="E230" s="109"/>
-      <c r="F230" s="109"/>
-      <c r="G230" s="41"/>
+      <c r="E230" s="70"/>
+      <c r="F230" s="70"/>
+      <c r="G230" s="39"/>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="58">
+      <c r="A231" s="53">
         <v>42955</v>
       </c>
-      <c r="B231" s="59">
+      <c r="B231" s="54">
         <v>1.06</v>
       </c>
       <c r="C231" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D231" s="109" t="s">
+      <c r="D231" s="70" t="s">
         <v>245</v>
       </c>
-      <c r="E231" s="109"/>
-      <c r="F231" s="109"/>
-      <c r="G231" s="41"/>
+      <c r="E231" s="70"/>
+      <c r="F231" s="70"/>
+      <c r="G231" s="39"/>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="58">
+      <c r="A232" s="53">
         <v>42991</v>
       </c>
-      <c r="B232" s="59">
+      <c r="B232" s="54">
         <v>1.07</v>
       </c>
       <c r="C232" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D232" s="109" t="s">
+      <c r="D232" s="70" t="s">
         <v>246</v>
       </c>
-      <c r="E232" s="109"/>
-      <c r="F232" s="109"/>
-      <c r="G232" s="41"/>
+      <c r="E232" s="70"/>
+      <c r="F232" s="70"/>
+      <c r="G232" s="39"/>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="58">
+      <c r="A233" s="53">
         <v>43026</v>
       </c>
-      <c r="B233" s="59">
+      <c r="B233" s="54">
         <v>1.08</v>
       </c>
       <c r="C233" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D233" s="109" t="s">
+      <c r="D233" s="70" t="s">
         <v>247</v>
       </c>
-      <c r="E233" s="109"/>
-      <c r="F233" s="109"/>
-      <c r="G233" s="41"/>
+      <c r="E233" s="70"/>
+      <c r="F233" s="70"/>
+      <c r="G233" s="39"/>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="58">
+      <c r="A234" s="53">
         <v>43069</v>
       </c>
-      <c r="B234" s="59">
+      <c r="B234" s="54">
         <v>1.0900000000000001</v>
       </c>
       <c r="C234" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D234" s="109" t="s">
+      <c r="D234" s="70" t="s">
         <v>248</v>
       </c>
-      <c r="E234" s="109"/>
-      <c r="F234" s="109"/>
-      <c r="G234" s="41"/>
+      <c r="E234" s="70"/>
+      <c r="F234" s="70"/>
+      <c r="G234" s="39"/>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="60">
+      <c r="A235" s="55">
         <v>43248</v>
       </c>
-      <c r="B235" s="61">
+      <c r="B235" s="56">
         <v>1.1000000000000001</v>
       </c>
       <c r="C235" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D235" s="105" t="s">
+      <c r="D235" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="E235" s="106"/>
-      <c r="F235" s="107"/>
-      <c r="G235" s="43"/>
+      <c r="E235" s="67"/>
+      <c r="F235" s="68"/>
+      <c r="G235" s="40"/>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="60">
+      <c r="A236" s="55">
         <v>43339</v>
       </c>
-      <c r="B236" s="61">
+      <c r="B236" s="56">
         <v>1.1100000000000001</v>
       </c>
       <c r="C236" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D236" s="105" t="s">
+      <c r="D236" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="E236" s="106"/>
-      <c r="F236" s="107"/>
-      <c r="G236" s="43"/>
+      <c r="E236" s="67"/>
+      <c r="F236" s="68"/>
+      <c r="G236" s="40"/>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="60">
+      <c r="A237" s="55">
         <v>43542</v>
       </c>
-      <c r="B237" s="61">
+      <c r="B237" s="56">
         <v>1.1200000000000001</v>
       </c>
       <c r="C237" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D237" s="105" t="s">
+      <c r="D237" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="E237" s="106"/>
-      <c r="F237" s="107"/>
-      <c r="G237" s="43"/>
+      <c r="E237" s="67"/>
+      <c r="F237" s="68"/>
+      <c r="G237" s="40"/>
     </row>
     <row r="238" spans="1:7">
-      <c r="A238" s="60">
+      <c r="A238" s="55">
         <v>43599</v>
       </c>
-      <c r="B238" s="61">
+      <c r="B238" s="56">
         <v>1.1299999999999999</v>
       </c>
       <c r="C238" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D238" s="62" t="s">
+      <c r="D238" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="E238" s="63"/>
-      <c r="F238" s="64"/>
-      <c r="G238" s="43"/>
+      <c r="E238" s="58"/>
+      <c r="F238" s="59"/>
+      <c r="G238" s="40"/>
     </row>
     <row r="239" spans="1:7">
-      <c r="A239" s="60">
+      <c r="A239" s="55">
         <v>43643</v>
       </c>
-      <c r="B239" s="61">
+      <c r="B239" s="56">
         <v>1.1399999999999999</v>
       </c>
       <c r="C239" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D239" s="62" t="s">
+      <c r="D239" s="57" t="s">
         <v>73</v>
       </c>
-      <c r="E239" s="63"/>
-      <c r="F239" s="64"/>
-      <c r="G239" s="43"/>
+      <c r="E239" s="58"/>
+      <c r="F239" s="59"/>
+      <c r="G239" s="40"/>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="60">
+      <c r="A240" s="55">
         <v>43894</v>
       </c>
-      <c r="B240" s="61">
+      <c r="B240" s="56">
         <v>1.1499999999999999</v>
       </c>
       <c r="C240" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D240" s="62" t="s">
+      <c r="D240" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="E240" s="63"/>
-      <c r="F240" s="64"/>
-      <c r="G240" s="43"/>
+      <c r="E240" s="58"/>
+      <c r="F240" s="59"/>
+      <c r="G240" s="40"/>
     </row>
     <row r="241" spans="1:7">
-      <c r="A241" s="60">
+      <c r="A241" s="55">
         <v>44017</v>
       </c>
-      <c r="B241" s="61">
+      <c r="B241" s="56">
         <v>1.1599999999999999</v>
       </c>
-      <c r="C241" s="42" t="s">
+      <c r="C241" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D241" s="62" t="s">
+      <c r="D241" s="57" t="s">
         <v>249</v>
       </c>
-      <c r="E241" s="63"/>
-      <c r="F241" s="64"/>
-      <c r="G241" s="43"/>
+      <c r="E241" s="58"/>
+      <c r="F241" s="59"/>
+      <c r="G241" s="40"/>
     </row>
     <row r="242" spans="1:7">
-      <c r="A242" s="60">
+      <c r="A242" s="55">
         <v>44118</v>
       </c>
-      <c r="B242" s="61">
+      <c r="B242" s="56">
         <v>1.17</v>
       </c>
-      <c r="C242" s="67" t="s">
+      <c r="C242" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="D242" s="62" t="s">
+      <c r="D242" s="57" t="s">
         <v>261</v>
       </c>
-      <c r="E242" s="63"/>
-      <c r="F242" s="64"/>
-      <c r="G242" s="43"/>
-    </row>
-    <row r="243" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A243" s="65">
+      <c r="E242" s="58"/>
+      <c r="F242" s="59"/>
+      <c r="G242" s="40"/>
+    </row>
+    <row r="243" spans="1:7" ht="15" thickBot="1">
+      <c r="A243" s="60">
         <v>44209</v>
       </c>
-      <c r="B243" s="66">
+      <c r="B243" s="61">
         <v>1.18</v>
       </c>
       <c r="C243" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D243" s="108" t="s">
+      <c r="D243" s="69" t="s">
         <v>264</v>
       </c>
-      <c r="E243" s="108"/>
-      <c r="F243" s="108"/>
-      <c r="G243" s="44"/>
+      <c r="E243" s="69"/>
+      <c r="F243" s="69"/>
+      <c r="G243" s="41"/>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}" scale="115">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="D236:F236"/>
-    <mergeCell ref="D237:F237"/>
-    <mergeCell ref="D243:F243"/>
-    <mergeCell ref="D230:F230"/>
-    <mergeCell ref="D231:F231"/>
-    <mergeCell ref="D232:F232"/>
-    <mergeCell ref="D233:F233"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="D229:F229"/>
-    <mergeCell ref="A212:A215"/>
-    <mergeCell ref="B212:B213"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="B214:B215"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="B222:E222"/>
-    <mergeCell ref="B223:E223"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="A208:A211"/>
-    <mergeCell ref="B208:B209"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="B210:B211"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="B174:B176"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="B148:B160"/>
+    <mergeCell ref="B161:B162"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="B166:B173"/>
     <mergeCell ref="B177:B178"/>
     <mergeCell ref="B179:B185"/>
     <mergeCell ref="C199:E199"/>
@@ -14710,12 +14684,35 @@
     <mergeCell ref="B206:B207"/>
     <mergeCell ref="C206:E206"/>
     <mergeCell ref="C207:E207"/>
-    <mergeCell ref="B174:B176"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="B148:B160"/>
-    <mergeCell ref="B161:B162"/>
-    <mergeCell ref="B163:B165"/>
-    <mergeCell ref="B166:B173"/>
+    <mergeCell ref="A208:A211"/>
+    <mergeCell ref="B208:B209"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="B210:B211"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="D229:F229"/>
+    <mergeCell ref="A212:A215"/>
+    <mergeCell ref="B212:B213"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="B214:B215"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="B222:E222"/>
+    <mergeCell ref="B223:E223"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="D236:F236"/>
+    <mergeCell ref="D237:F237"/>
+    <mergeCell ref="D243:F243"/>
+    <mergeCell ref="D230:F230"/>
+    <mergeCell ref="D231:F231"/>
+    <mergeCell ref="D232:F232"/>
+    <mergeCell ref="D233:F233"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -14724,12 +14721,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -14738,18 +14735,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{3E5CE8AE-B586-4A12-8744-B7D8B6DA7A89}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
f101--avant dsp suite added
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_12_Avant_GX.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_12_Avant_GX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795A234F-A4DF-4F33-91FD-9BD926D50B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833FEB0D-F444-42BB-A155-E963B03B8FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,16 +34,16 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2" showComments="commIndAndComment"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Jeffrey Ye - Personal View" guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2" showComments="commIndAndComment"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4189" uniqueCount="1330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4194" uniqueCount="1330">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -5080,67 +5080,38 @@
     <xf numFmtId="49" fontId="9" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
@@ -5163,26 +5134,55 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -8063,7 +8063,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8336,8 +8336,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
-      <selection activeCell="G17" sqref="G17"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B13" sqref="B13"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -8346,13 +8351,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B13" sqref="B13"/>
+    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
+      <selection activeCell="G17" sqref="G17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -8370,7 +8370,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C62" sqref="C62"/>
+      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -9613,6 +9613,9 @@
     <row r="42" spans="1:32">
       <c r="A42" s="73" t="s">
         <v>302</v>
+      </c>
+      <c r="B42" s="53" t="s">
+        <v>39</v>
       </c>
       <c r="C42" s="53" t="s">
         <v>1204</v>
@@ -10631,10 +10634,10 @@
   <dimension ref="A1:AF194"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B173" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Y186" sqref="Y186"/>
+      <selection pane="bottomRight" activeCell="C196" sqref="C196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -14226,6 +14229,9 @@
       <c r="A97" s="53" t="s">
         <v>1223</v>
       </c>
+      <c r="B97" s="53" t="s">
+        <v>39</v>
+      </c>
       <c r="C97" s="53" t="s">
         <v>919</v>
       </c>
@@ -14255,6 +14261,9 @@
       <c r="A98" s="53" t="s">
         <v>1224</v>
       </c>
+      <c r="B98" s="53" t="s">
+        <v>39</v>
+      </c>
       <c r="C98" s="53" t="s">
         <v>920</v>
       </c>
@@ -17910,6 +17919,9 @@
       <c r="A193" s="53" t="s">
         <v>1319</v>
       </c>
+      <c r="B193" s="53" t="s">
+        <v>39</v>
+      </c>
       <c r="C193" s="53" t="s">
         <v>1049</v>
       </c>
@@ -17938,6 +17950,9 @@
     <row r="194" spans="1:32">
       <c r="A194" s="53" t="s">
         <v>1320</v>
+      </c>
+      <c r="B194" s="53" t="s">
+        <v>39</v>
       </c>
       <c r="C194" s="53" t="s">
         <v>1050</v>
@@ -18108,17 +18123,17 @@
       <c r="E111" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F111" s="112" t="s">
+      <c r="F111" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="G111" s="113"/>
-      <c r="H111" s="113"/>
-      <c r="I111" s="113"/>
-      <c r="J111" s="113"/>
-      <c r="K111" s="113"/>
-      <c r="L111" s="113"/>
-      <c r="M111" s="113"/>
-      <c r="N111" s="114"/>
+      <c r="G111" s="144"/>
+      <c r="H111" s="144"/>
+      <c r="I111" s="144"/>
+      <c r="J111" s="144"/>
+      <c r="K111" s="144"/>
+      <c r="L111" s="144"/>
+      <c r="M111" s="144"/>
+      <c r="N111" s="145"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -19038,7 +19053,7 @@
       <c r="A149" s="19">
         <v>1</v>
       </c>
-      <c r="B149" s="143" t="s">
+      <c r="B149" s="112" t="s">
         <v>3</v>
       </c>
       <c r="C149" s="56" t="s">
@@ -19064,7 +19079,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="144"/>
+      <c r="B150" s="114"/>
       <c r="C150" s="21" t="s">
         <v>81</v>
       </c>
@@ -19086,7 +19101,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="144"/>
+      <c r="B151" s="114"/>
       <c r="C151" s="21" t="s">
         <v>16</v>
       </c>
@@ -19106,7 +19121,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="144"/>
+      <c r="B152" s="114"/>
       <c r="C152" s="21" t="s">
         <v>83</v>
       </c>
@@ -19130,7 +19145,7 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="144"/>
+      <c r="B153" s="114"/>
       <c r="C153" s="56" t="s">
         <v>85</v>
       </c>
@@ -19154,7 +19169,7 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="144"/>
+      <c r="B154" s="114"/>
       <c r="C154" s="56" t="s">
         <v>89</v>
       </c>
@@ -19178,7 +19193,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="144"/>
+      <c r="B155" s="114"/>
       <c r="C155" s="21" t="s">
         <v>91</v>
       </c>
@@ -19200,7 +19215,7 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="144"/>
+      <c r="B156" s="114"/>
       <c r="C156" s="56" t="s">
         <v>92</v>
       </c>
@@ -19224,7 +19239,7 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="144"/>
+      <c r="B157" s="114"/>
       <c r="C157" s="56" t="s">
         <v>93</v>
       </c>
@@ -19248,7 +19263,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="144"/>
+      <c r="B158" s="114"/>
       <c r="C158" s="21" t="s">
         <v>94</v>
       </c>
@@ -19272,7 +19287,7 @@
       <c r="A159" s="19">
         <v>11</v>
       </c>
-      <c r="B159" s="144"/>
+      <c r="B159" s="114"/>
       <c r="C159" s="21" t="s">
         <v>95</v>
       </c>
@@ -19296,7 +19311,7 @@
       <c r="A160" s="19">
         <v>12</v>
       </c>
-      <c r="B160" s="144"/>
+      <c r="B160" s="114"/>
       <c r="C160" s="21" t="s">
         <v>97</v>
       </c>
@@ -19318,7 +19333,7 @@
       <c r="A161" s="19">
         <v>13</v>
       </c>
-      <c r="B161" s="129"/>
+      <c r="B161" s="121"/>
       <c r="C161" s="21" t="s">
         <v>101</v>
       </c>
@@ -19342,7 +19357,7 @@
       <c r="A162" s="19">
         <v>14</v>
       </c>
-      <c r="B162" s="124" t="s">
+      <c r="B162" s="122" t="s">
         <v>4</v>
       </c>
       <c r="C162" s="21" t="s">
@@ -19368,7 +19383,7 @@
       <c r="A163" s="19">
         <v>15</v>
       </c>
-      <c r="B163" s="125"/>
+      <c r="B163" s="119"/>
       <c r="C163" s="21" t="s">
         <v>108</v>
       </c>
@@ -19392,7 +19407,7 @@
       <c r="A164" s="19">
         <v>16</v>
       </c>
-      <c r="B164" s="143" t="s">
+      <c r="B164" s="112" t="s">
         <v>5</v>
       </c>
       <c r="C164" s="21" t="s">
@@ -19416,7 +19431,7 @@
       <c r="A165" s="19">
         <v>17</v>
       </c>
-      <c r="B165" s="145"/>
+      <c r="B165" s="113"/>
       <c r="C165" s="56" t="s">
         <v>212</v>
       </c>
@@ -19438,7 +19453,7 @@
       <c r="A166" s="19">
         <v>18</v>
       </c>
-      <c r="B166" s="129"/>
+      <c r="B166" s="121"/>
       <c r="C166" s="56" t="s">
         <v>112</v>
       </c>
@@ -19458,7 +19473,7 @@
       <c r="A167" s="19">
         <v>19</v>
       </c>
-      <c r="B167" s="124" t="s">
+      <c r="B167" s="122" t="s">
         <v>6</v>
       </c>
       <c r="C167" s="21" t="s">
@@ -19482,7 +19497,7 @@
       <c r="A168" s="19">
         <v>20</v>
       </c>
-      <c r="B168" s="125"/>
+      <c r="B168" s="119"/>
       <c r="C168" s="21" t="s">
         <v>117</v>
       </c>
@@ -19502,7 +19517,7 @@
       <c r="A169" s="19">
         <v>21</v>
       </c>
-      <c r="B169" s="125"/>
+      <c r="B169" s="119"/>
       <c r="C169" s="21" t="s">
         <v>118</v>
       </c>
@@ -19522,7 +19537,7 @@
       <c r="A170" s="19">
         <v>22</v>
       </c>
-      <c r="B170" s="125"/>
+      <c r="B170" s="119"/>
       <c r="C170" s="21" t="s">
         <v>119</v>
       </c>
@@ -19542,7 +19557,7 @@
       <c r="A171" s="19">
         <v>23</v>
       </c>
-      <c r="B171" s="125"/>
+      <c r="B171" s="119"/>
       <c r="C171" s="21" t="s">
         <v>120</v>
       </c>
@@ -19562,7 +19577,7 @@
       <c r="A172" s="19">
         <v>24</v>
       </c>
-      <c r="B172" s="125"/>
+      <c r="B172" s="119"/>
       <c r="C172" s="21" t="s">
         <v>121</v>
       </c>
@@ -19582,7 +19597,7 @@
       <c r="A173" s="19">
         <v>25</v>
       </c>
-      <c r="B173" s="125"/>
+      <c r="B173" s="119"/>
       <c r="C173" s="21" t="s">
         <v>122</v>
       </c>
@@ -19602,7 +19617,7 @@
       <c r="A174" s="19">
         <v>26</v>
       </c>
-      <c r="B174" s="125"/>
+      <c r="B174" s="119"/>
       <c r="C174" s="21" t="s">
         <v>38</v>
       </c>
@@ -19622,7 +19637,7 @@
       <c r="A175" s="19">
         <v>27</v>
       </c>
-      <c r="B175" s="124" t="s">
+      <c r="B175" s="122" t="s">
         <v>7</v>
       </c>
       <c r="C175" s="21" t="s">
@@ -19646,7 +19661,7 @@
       <c r="A176" s="19">
         <v>28</v>
       </c>
-      <c r="B176" s="125"/>
+      <c r="B176" s="119"/>
       <c r="C176" s="56" t="s">
         <v>124</v>
       </c>
@@ -19668,7 +19683,7 @@
       <c r="A177" s="19">
         <v>29</v>
       </c>
-      <c r="B177" s="125"/>
+      <c r="B177" s="119"/>
       <c r="C177" s="56" t="s">
         <v>237</v>
       </c>
@@ -19690,7 +19705,7 @@
       <c r="A178" s="19">
         <v>30</v>
       </c>
-      <c r="B178" s="125"/>
+      <c r="B178" s="119"/>
       <c r="C178" s="56" t="s">
         <v>127</v>
       </c>
@@ -19712,7 +19727,7 @@
       <c r="A179" s="19">
         <v>31</v>
       </c>
-      <c r="B179" s="125"/>
+      <c r="B179" s="119"/>
       <c r="C179" s="56" t="s">
         <v>234</v>
       </c>
@@ -19734,7 +19749,7 @@
       <c r="A180" s="19">
         <v>32</v>
       </c>
-      <c r="B180" s="125"/>
+      <c r="B180" s="119"/>
       <c r="C180" s="56" t="s">
         <v>235</v>
       </c>
@@ -19756,7 +19771,7 @@
       <c r="A181" s="19">
         <v>33</v>
       </c>
-      <c r="B181" s="143" t="s">
+      <c r="B181" s="112" t="s">
         <v>8</v>
       </c>
       <c r="C181" s="21" t="s">
@@ -19782,7 +19797,7 @@
       <c r="A182" s="22">
         <v>34</v>
       </c>
-      <c r="B182" s="145"/>
+      <c r="B182" s="113"/>
       <c r="C182" s="20" t="s">
         <v>131</v>
       </c>
@@ -19806,7 +19821,7 @@
       <c r="A183" s="22">
         <v>35</v>
       </c>
-      <c r="B183" s="144"/>
+      <c r="B183" s="114"/>
       <c r="C183" s="58" t="s">
         <v>240</v>
       </c>
@@ -19830,7 +19845,7 @@
       <c r="A184" s="16">
         <v>36</v>
       </c>
-      <c r="B184" s="146" t="s">
+      <c r="B184" s="115" t="s">
         <v>64</v>
       </c>
       <c r="C184" s="57" t="s">
@@ -19854,7 +19869,7 @@
       <c r="A185" s="19">
         <v>37</v>
       </c>
-      <c r="B185" s="147"/>
+      <c r="B185" s="116"/>
       <c r="C185" s="56" t="s">
         <v>136</v>
       </c>
@@ -19876,7 +19891,7 @@
       <c r="A186" s="19">
         <v>38</v>
       </c>
-      <c r="B186" s="148"/>
+      <c r="B186" s="117"/>
       <c r="C186" s="58" t="s">
         <v>139</v>
       </c>
@@ -19898,7 +19913,7 @@
       <c r="A187" s="19">
         <v>39</v>
       </c>
-      <c r="B187" s="148"/>
+      <c r="B187" s="117"/>
       <c r="C187" s="58" t="s">
         <v>140</v>
       </c>
@@ -19920,7 +19935,7 @@
       <c r="A188" s="19">
         <v>40</v>
       </c>
-      <c r="B188" s="148"/>
+      <c r="B188" s="117"/>
       <c r="C188" s="58" t="s">
         <v>143</v>
       </c>
@@ -19940,7 +19955,7 @@
       <c r="A189" s="19">
         <v>41</v>
       </c>
-      <c r="B189" s="148"/>
+      <c r="B189" s="117"/>
       <c r="C189" s="58" t="s">
         <v>219</v>
       </c>
@@ -19962,7 +19977,7 @@
       <c r="A190" s="24">
         <v>42</v>
       </c>
-      <c r="B190" s="133"/>
+      <c r="B190" s="118"/>
       <c r="C190" s="25" t="s">
         <v>223</v>
       </c>
@@ -20013,11 +20028,11 @@
       <c r="B204" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="C204" s="115" t="s">
+      <c r="C204" s="146" t="s">
         <v>151</v>
       </c>
-      <c r="D204" s="115"/>
-      <c r="E204" s="115"/>
+      <c r="D204" s="146"/>
+      <c r="E204" s="146"/>
       <c r="F204" s="27" t="s">
         <v>152</v>
       </c>
@@ -20026,17 +20041,17 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="141" t="s">
+      <c r="A205" s="128" t="s">
         <v>154</v>
       </c>
-      <c r="B205" s="125" t="s">
+      <c r="B205" s="119" t="s">
         <v>155</v>
       </c>
-      <c r="C205" s="116" t="s">
+      <c r="C205" s="147" t="s">
         <v>156</v>
       </c>
-      <c r="D205" s="117"/>
-      <c r="E205" s="117"/>
+      <c r="D205" s="148"/>
+      <c r="E205" s="148"/>
       <c r="F205" s="21" t="s">
         <v>157</v>
       </c>
@@ -20045,13 +20060,13 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="141"/>
-      <c r="B206" s="149"/>
-      <c r="C206" s="118" t="s">
+      <c r="A206" s="128"/>
+      <c r="B206" s="120"/>
+      <c r="C206" s="138" t="s">
         <v>156</v>
       </c>
-      <c r="D206" s="119"/>
-      <c r="E206" s="119"/>
+      <c r="D206" s="149"/>
+      <c r="E206" s="149"/>
       <c r="F206" s="20" t="s">
         <v>159</v>
       </c>
@@ -20060,15 +20075,15 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="141"/>
-      <c r="B207" s="125" t="s">
+      <c r="A207" s="128"/>
+      <c r="B207" s="119" t="s">
         <v>160</v>
       </c>
-      <c r="C207" s="120" t="s">
+      <c r="C207" s="142" t="s">
         <v>161</v>
       </c>
-      <c r="D207" s="120"/>
-      <c r="E207" s="120"/>
+      <c r="D207" s="142"/>
+      <c r="E207" s="142"/>
       <c r="F207" s="21" t="s">
         <v>157</v>
       </c>
@@ -20077,13 +20092,13 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="141"/>
-      <c r="B208" s="125"/>
-      <c r="C208" s="118" t="s">
+      <c r="A208" s="128"/>
+      <c r="B208" s="119"/>
+      <c r="C208" s="138" t="s">
         <v>161</v>
       </c>
-      <c r="D208" s="118"/>
-      <c r="E208" s="118"/>
+      <c r="D208" s="138"/>
+      <c r="E208" s="138"/>
       <c r="F208" s="21" t="s">
         <v>159</v>
       </c>
@@ -20092,15 +20107,15 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="141"/>
-      <c r="B209" s="149" t="s">
+      <c r="A209" s="128"/>
+      <c r="B209" s="120" t="s">
         <v>162</v>
       </c>
-      <c r="C209" s="121" t="s">
+      <c r="C209" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="D209" s="122"/>
-      <c r="E209" s="123"/>
+      <c r="D209" s="140"/>
+      <c r="E209" s="141"/>
       <c r="F209" s="21" t="s">
         <v>157</v>
       </c>
@@ -20109,13 +20124,13 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="141"/>
-      <c r="B210" s="129"/>
-      <c r="C210" s="121" t="s">
+      <c r="A210" s="128"/>
+      <c r="B210" s="121"/>
+      <c r="C210" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="D210" s="122"/>
-      <c r="E210" s="123"/>
+      <c r="D210" s="140"/>
+      <c r="E210" s="141"/>
       <c r="F210" s="21" t="s">
         <v>159</v>
       </c>
@@ -20124,15 +20139,15 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="141"/>
-      <c r="B211" s="125" t="s">
+      <c r="A211" s="128"/>
+      <c r="B211" s="119" t="s">
         <v>163</v>
       </c>
-      <c r="C211" s="120" t="s">
+      <c r="C211" s="142" t="s">
         <v>164</v>
       </c>
-      <c r="D211" s="120"/>
-      <c r="E211" s="120"/>
+      <c r="D211" s="142"/>
+      <c r="E211" s="142"/>
       <c r="F211" s="21" t="s">
         <v>157</v>
       </c>
@@ -20141,13 +20156,13 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="141"/>
-      <c r="B212" s="125"/>
-      <c r="C212" s="120" t="s">
+      <c r="A212" s="128"/>
+      <c r="B212" s="119"/>
+      <c r="C212" s="142" t="s">
         <v>164</v>
       </c>
-      <c r="D212" s="120"/>
-      <c r="E212" s="120"/>
+      <c r="D212" s="142"/>
+      <c r="E212" s="142"/>
       <c r="F212" s="21" t="s">
         <v>159</v>
       </c>
@@ -20156,17 +20171,17 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="141" t="s">
+      <c r="A213" s="128" t="s">
         <v>165</v>
       </c>
-      <c r="B213" s="125" t="s">
+      <c r="B213" s="119" t="s">
         <v>166</v>
       </c>
-      <c r="C213" s="124" t="s">
+      <c r="C213" s="122" t="s">
         <v>167</v>
       </c>
-      <c r="D213" s="125"/>
-      <c r="E213" s="125"/>
+      <c r="D213" s="119"/>
+      <c r="E213" s="119"/>
       <c r="F213" s="21" t="s">
         <v>157</v>
       </c>
@@ -20175,13 +20190,13 @@
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="141"/>
-      <c r="B214" s="125"/>
-      <c r="C214" s="125" t="s">
+      <c r="A214" s="128"/>
+      <c r="B214" s="119"/>
+      <c r="C214" s="119" t="s">
         <v>168</v>
       </c>
-      <c r="D214" s="125"/>
-      <c r="E214" s="125"/>
+      <c r="D214" s="119"/>
+      <c r="E214" s="119"/>
       <c r="F214" s="21" t="s">
         <v>159</v>
       </c>
@@ -20190,15 +20205,15 @@
       </c>
     </row>
     <row r="215" spans="1:7">
-      <c r="A215" s="141"/>
-      <c r="B215" s="125" t="s">
+      <c r="A215" s="128"/>
+      <c r="B215" s="119" t="s">
         <v>170</v>
       </c>
-      <c r="C215" s="125" t="s">
+      <c r="C215" s="119" t="s">
         <v>171</v>
       </c>
-      <c r="D215" s="125"/>
-      <c r="E215" s="125"/>
+      <c r="D215" s="119"/>
+      <c r="E215" s="119"/>
       <c r="F215" s="21" t="s">
         <v>157</v>
       </c>
@@ -20207,13 +20222,13 @@
       </c>
     </row>
     <row r="216" spans="1:7">
-      <c r="A216" s="141"/>
-      <c r="B216" s="125"/>
-      <c r="C216" s="125" t="s">
+      <c r="A216" s="128"/>
+      <c r="B216" s="119"/>
+      <c r="C216" s="119" t="s">
         <v>172</v>
       </c>
-      <c r="D216" s="125"/>
-      <c r="E216" s="125"/>
+      <c r="D216" s="119"/>
+      <c r="E216" s="119"/>
       <c r="F216" s="21" t="s">
         <v>159</v>
       </c>
@@ -20222,17 +20237,17 @@
       </c>
     </row>
     <row r="217" spans="1:7">
-      <c r="A217" s="141" t="s">
+      <c r="A217" s="128" t="s">
         <v>173</v>
       </c>
-      <c r="B217" s="125" t="s">
+      <c r="B217" s="119" t="s">
         <v>174</v>
       </c>
-      <c r="C217" s="124" t="s">
+      <c r="C217" s="122" t="s">
         <v>175</v>
       </c>
-      <c r="D217" s="125"/>
-      <c r="E217" s="125"/>
+      <c r="D217" s="119"/>
+      <c r="E217" s="119"/>
       <c r="F217" s="21" t="s">
         <v>157</v>
       </c>
@@ -20241,13 +20256,13 @@
       </c>
     </row>
     <row r="218" spans="1:7">
-      <c r="A218" s="141"/>
-      <c r="B218" s="125"/>
-      <c r="C218" s="125" t="s">
+      <c r="A218" s="128"/>
+      <c r="B218" s="119"/>
+      <c r="C218" s="119" t="s">
         <v>176</v>
       </c>
-      <c r="D218" s="125"/>
-      <c r="E218" s="125"/>
+      <c r="D218" s="119"/>
+      <c r="E218" s="119"/>
       <c r="F218" s="21" t="s">
         <v>159</v>
       </c>
@@ -20256,15 +20271,15 @@
       </c>
     </row>
     <row r="219" spans="1:7">
-      <c r="A219" s="141"/>
-      <c r="B219" s="125" t="s">
+      <c r="A219" s="128"/>
+      <c r="B219" s="119" t="s">
         <v>177</v>
       </c>
-      <c r="C219" s="124" t="s">
+      <c r="C219" s="122" t="s">
         <v>178</v>
       </c>
-      <c r="D219" s="125"/>
-      <c r="E219" s="125"/>
+      <c r="D219" s="119"/>
+      <c r="E219" s="119"/>
       <c r="F219" s="21" t="s">
         <v>157</v>
       </c>
@@ -20273,13 +20288,13 @@
       </c>
     </row>
     <row r="220" spans="1:7">
-      <c r="A220" s="142"/>
-      <c r="B220" s="126"/>
-      <c r="C220" s="126" t="s">
+      <c r="A220" s="129"/>
+      <c r="B220" s="130"/>
+      <c r="C220" s="130" t="s">
         <v>179</v>
       </c>
-      <c r="D220" s="126"/>
-      <c r="E220" s="126"/>
+      <c r="D220" s="130"/>
+      <c r="E220" s="130"/>
       <c r="F220" s="25" t="s">
         <v>159</v>
       </c>
@@ -20301,12 +20316,12 @@
       <c r="A225" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="B225" s="127" t="s">
+      <c r="B225" s="136" t="s">
         <v>183</v>
       </c>
-      <c r="C225" s="127"/>
-      <c r="D225" s="127"/>
-      <c r="E225" s="127"/>
+      <c r="C225" s="136"/>
+      <c r="D225" s="136"/>
+      <c r="E225" s="136"/>
       <c r="F225" s="33" t="s">
         <v>184</v>
       </c>
@@ -20318,12 +20333,12 @@
       <c r="A226" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="B226" s="128" t="s">
+      <c r="B226" s="137" t="s">
         <v>187</v>
       </c>
-      <c r="C226" s="129"/>
-      <c r="D226" s="129"/>
-      <c r="E226" s="129"/>
+      <c r="C226" s="121"/>
+      <c r="D226" s="121"/>
+      <c r="E226" s="121"/>
       <c r="F226" s="36" t="s">
         <v>62</v>
       </c>
@@ -20335,12 +20350,12 @@
       <c r="A227" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B227" s="130" t="s">
+      <c r="B227" s="132" t="s">
         <v>189</v>
       </c>
-      <c r="C227" s="131"/>
-      <c r="D227" s="131"/>
-      <c r="E227" s="132"/>
+      <c r="C227" s="133"/>
+      <c r="D227" s="133"/>
+      <c r="E227" s="134"/>
       <c r="F227" s="9" t="s">
         <v>158</v>
       </c>
@@ -20352,12 +20367,12 @@
       <c r="A228" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B228" s="130" t="s">
+      <c r="B228" s="132" t="s">
         <v>191</v>
       </c>
-      <c r="C228" s="131"/>
-      <c r="D228" s="131"/>
-      <c r="E228" s="132"/>
+      <c r="C228" s="133"/>
+      <c r="D228" s="133"/>
+      <c r="E228" s="134"/>
       <c r="F228" s="13" t="s">
         <v>158</v>
       </c>
@@ -20369,12 +20384,12 @@
       <c r="A229" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="B229" s="133" t="s">
+      <c r="B229" s="118" t="s">
         <v>193</v>
       </c>
-      <c r="C229" s="126"/>
-      <c r="D229" s="126"/>
-      <c r="E229" s="126"/>
+      <c r="C229" s="130"/>
+      <c r="D229" s="130"/>
+      <c r="E229" s="130"/>
       <c r="F229" s="15" t="s">
         <v>158</v>
       </c>
@@ -20419,11 +20434,11 @@
       <c r="C234" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="D234" s="134" t="s">
+      <c r="D234" s="135" t="s">
         <v>199</v>
       </c>
-      <c r="E234" s="134"/>
-      <c r="F234" s="134"/>
+      <c r="E234" s="135"/>
+      <c r="F234" s="135"/>
       <c r="G234" s="18"/>
     </row>
     <row r="235" spans="1:7">
@@ -20436,11 +20451,11 @@
       <c r="C235" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D235" s="135" t="s">
+      <c r="D235" s="131" t="s">
         <v>200</v>
       </c>
-      <c r="E235" s="135"/>
-      <c r="F235" s="135"/>
+      <c r="E235" s="131"/>
+      <c r="F235" s="131"/>
       <c r="G235" s="29"/>
     </row>
     <row r="236" spans="1:7">
@@ -20453,11 +20468,11 @@
       <c r="C236" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D236" s="135" t="s">
+      <c r="D236" s="131" t="s">
         <v>201</v>
       </c>
-      <c r="E236" s="135"/>
-      <c r="F236" s="135"/>
+      <c r="E236" s="131"/>
+      <c r="F236" s="131"/>
       <c r="G236" s="29"/>
     </row>
     <row r="237" spans="1:7">
@@ -20470,11 +20485,11 @@
       <c r="C237" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D237" s="135" t="s">
+      <c r="D237" s="131" t="s">
         <v>202</v>
       </c>
-      <c r="E237" s="135"/>
-      <c r="F237" s="135"/>
+      <c r="E237" s="131"/>
+      <c r="F237" s="131"/>
       <c r="G237" s="29"/>
     </row>
     <row r="238" spans="1:7">
@@ -20487,11 +20502,11 @@
       <c r="C238" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D238" s="135" t="s">
+      <c r="D238" s="131" t="s">
         <v>203</v>
       </c>
-      <c r="E238" s="135"/>
-      <c r="F238" s="135"/>
+      <c r="E238" s="131"/>
+      <c r="F238" s="131"/>
       <c r="G238" s="29"/>
     </row>
     <row r="239" spans="1:7">
@@ -20504,11 +20519,11 @@
       <c r="C239" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D239" s="135" t="s">
+      <c r="D239" s="131" t="s">
         <v>204</v>
       </c>
-      <c r="E239" s="135"/>
-      <c r="F239" s="135"/>
+      <c r="E239" s="131"/>
+      <c r="F239" s="131"/>
       <c r="G239" s="29"/>
     </row>
     <row r="240" spans="1:7">
@@ -20521,11 +20536,11 @@
       <c r="C240" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="D240" s="136" t="s">
+      <c r="D240" s="123" t="s">
         <v>205</v>
       </c>
-      <c r="E240" s="137"/>
-      <c r="F240" s="138"/>
+      <c r="E240" s="124"/>
+      <c r="F240" s="125"/>
       <c r="G240" s="30"/>
     </row>
     <row r="241" spans="1:7">
@@ -20538,11 +20553,11 @@
       <c r="C241" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="D241" s="136" t="s">
+      <c r="D241" s="123" t="s">
         <v>206</v>
       </c>
-      <c r="E241" s="137"/>
-      <c r="F241" s="138"/>
+      <c r="E241" s="124"/>
+      <c r="F241" s="125"/>
       <c r="G241" s="30"/>
     </row>
     <row r="242" spans="1:7">
@@ -20555,11 +20570,11 @@
       <c r="C242" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="D242" s="136" t="s">
+      <c r="D242" s="123" t="s">
         <v>207</v>
       </c>
-      <c r="E242" s="137"/>
-      <c r="F242" s="138"/>
+      <c r="E242" s="124"/>
+      <c r="F242" s="125"/>
       <c r="G242" s="30"/>
     </row>
     <row r="243" spans="1:7">
@@ -20708,36 +20723,51 @@
       <c r="C251" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="D251" s="139" t="s">
+      <c r="D251" s="126" t="s">
         <v>245</v>
       </c>
-      <c r="E251" s="140"/>
-      <c r="F251" s="140"/>
+      <c r="E251" s="127"/>
+      <c r="F251" s="127"/>
       <c r="G251" s="31"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Y3CbQBUOESlDRywGeoG/3StrDbFnCkeqkNskZfEB2tOROsi5KmkcJgzaGARx/t71p+8XW8S30YXLCnas8V4vyw==" saltValue="Hjy+0Aja5MmvK1SBdUhEOA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}" scale="115">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}" scale="115">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B181:B183"/>
-    <mergeCell ref="B184:B190"/>
-    <mergeCell ref="B205:B206"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="B149:B161"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="B164:B166"/>
-    <mergeCell ref="B167:B174"/>
-    <mergeCell ref="B175:B180"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C204:E204"/>
+    <mergeCell ref="C205:E205"/>
+    <mergeCell ref="C206:E206"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="C216:E216"/>
+    <mergeCell ref="C217:E217"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C219:E219"/>
+    <mergeCell ref="C220:E220"/>
+    <mergeCell ref="B225:E225"/>
+    <mergeCell ref="B226:E226"/>
+    <mergeCell ref="B227:E227"/>
+    <mergeCell ref="B228:E228"/>
+    <mergeCell ref="B229:E229"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
     <mergeCell ref="D241:F241"/>
     <mergeCell ref="D242:F242"/>
     <mergeCell ref="D251:F251"/>
@@ -20754,31 +20784,16 @@
     <mergeCell ref="D238:F238"/>
     <mergeCell ref="D239:F239"/>
     <mergeCell ref="D240:F240"/>
-    <mergeCell ref="B227:E227"/>
-    <mergeCell ref="B228:E228"/>
-    <mergeCell ref="B229:E229"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="C219:E219"/>
-    <mergeCell ref="C220:E220"/>
-    <mergeCell ref="B225:E225"/>
-    <mergeCell ref="B226:E226"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="C216:E216"/>
-    <mergeCell ref="C217:E217"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="C205:E205"/>
-    <mergeCell ref="C206:E206"/>
-    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="B149:B161"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="B164:B166"/>
+    <mergeCell ref="B167:B174"/>
+    <mergeCell ref="B175:B180"/>
+    <mergeCell ref="B181:B183"/>
+    <mergeCell ref="B184:B190"/>
+    <mergeCell ref="B205:B206"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="B209:B210"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -23623,19 +23638,19 @@
   </sheetData>
   <autoFilter ref="B1:J97" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <customSheetViews>
-    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <selection activeCell="D24" sqref="D24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
       <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>

<commit_message>
i480--Add design name in output log
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_12_Avant_GX.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_12_Avant_GX.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwang1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833FEB0D-F444-42BB-A155-E963B03B8FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD89189A-F219-4E2A-A43D-70FEBB1F8D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,16 +34,16 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jeffrey Ye - Personal View" guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2" showComments="commIndAndComment"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Jeffrey Ye - Personal View" guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4194" uniqueCount="1330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4193" uniqueCount="1330">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -5080,38 +5080,67 @@
     <xf numFmtId="49" fontId="9" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
@@ -5134,55 +5163,26 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -8063,7 +8063,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8336,8 +8336,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B13" sqref="B13"/>
+    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
+      <selection activeCell="G17" sqref="G17"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -8346,13 +8351,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait"/>
-    </customSheetView>
-    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
-      <selection activeCell="G17" sqref="G17"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -8370,7 +8370,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
+      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -9613,9 +9613,6 @@
     <row r="42" spans="1:32">
       <c r="A42" s="73" t="s">
         <v>302</v>
-      </c>
-      <c r="B42" s="53" t="s">
-        <v>39</v>
       </c>
       <c r="C42" s="53" t="s">
         <v>1204</v>
@@ -18062,7 +18059,7 @@
   <dimension ref="A1:N251"/>
   <sheetViews>
     <sheetView topLeftCell="A190" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D255" sqref="D255"/>
+      <selection activeCell="C219" sqref="C219:E219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -18123,17 +18120,17 @@
       <c r="E111" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F111" s="143" t="s">
+      <c r="F111" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="G111" s="144"/>
-      <c r="H111" s="144"/>
-      <c r="I111" s="144"/>
-      <c r="J111" s="144"/>
-      <c r="K111" s="144"/>
-      <c r="L111" s="144"/>
-      <c r="M111" s="144"/>
-      <c r="N111" s="145"/>
+      <c r="G111" s="113"/>
+      <c r="H111" s="113"/>
+      <c r="I111" s="113"/>
+      <c r="J111" s="113"/>
+      <c r="K111" s="113"/>
+      <c r="L111" s="113"/>
+      <c r="M111" s="113"/>
+      <c r="N111" s="114"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -19053,7 +19050,7 @@
       <c r="A149" s="19">
         <v>1</v>
       </c>
-      <c r="B149" s="112" t="s">
+      <c r="B149" s="143" t="s">
         <v>3</v>
       </c>
       <c r="C149" s="56" t="s">
@@ -19079,7 +19076,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="114"/>
+      <c r="B150" s="144"/>
       <c r="C150" s="21" t="s">
         <v>81</v>
       </c>
@@ -19101,7 +19098,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="114"/>
+      <c r="B151" s="144"/>
       <c r="C151" s="21" t="s">
         <v>16</v>
       </c>
@@ -19121,7 +19118,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="114"/>
+      <c r="B152" s="144"/>
       <c r="C152" s="21" t="s">
         <v>83</v>
       </c>
@@ -19145,7 +19142,7 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="114"/>
+      <c r="B153" s="144"/>
       <c r="C153" s="56" t="s">
         <v>85</v>
       </c>
@@ -19169,7 +19166,7 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="114"/>
+      <c r="B154" s="144"/>
       <c r="C154" s="56" t="s">
         <v>89</v>
       </c>
@@ -19193,7 +19190,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="114"/>
+      <c r="B155" s="144"/>
       <c r="C155" s="21" t="s">
         <v>91</v>
       </c>
@@ -19215,7 +19212,7 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="114"/>
+      <c r="B156" s="144"/>
       <c r="C156" s="56" t="s">
         <v>92</v>
       </c>
@@ -19239,7 +19236,7 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="114"/>
+      <c r="B157" s="144"/>
       <c r="C157" s="56" t="s">
         <v>93</v>
       </c>
@@ -19263,7 +19260,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="114"/>
+      <c r="B158" s="144"/>
       <c r="C158" s="21" t="s">
         <v>94</v>
       </c>
@@ -19287,7 +19284,7 @@
       <c r="A159" s="19">
         <v>11</v>
       </c>
-      <c r="B159" s="114"/>
+      <c r="B159" s="144"/>
       <c r="C159" s="21" t="s">
         <v>95</v>
       </c>
@@ -19311,7 +19308,7 @@
       <c r="A160" s="19">
         <v>12</v>
       </c>
-      <c r="B160" s="114"/>
+      <c r="B160" s="144"/>
       <c r="C160" s="21" t="s">
         <v>97</v>
       </c>
@@ -19333,7 +19330,7 @@
       <c r="A161" s="19">
         <v>13</v>
       </c>
-      <c r="B161" s="121"/>
+      <c r="B161" s="129"/>
       <c r="C161" s="21" t="s">
         <v>101</v>
       </c>
@@ -19357,7 +19354,7 @@
       <c r="A162" s="19">
         <v>14</v>
       </c>
-      <c r="B162" s="122" t="s">
+      <c r="B162" s="124" t="s">
         <v>4</v>
       </c>
       <c r="C162" s="21" t="s">
@@ -19383,7 +19380,7 @@
       <c r="A163" s="19">
         <v>15</v>
       </c>
-      <c r="B163" s="119"/>
+      <c r="B163" s="125"/>
       <c r="C163" s="21" t="s">
         <v>108</v>
       </c>
@@ -19407,7 +19404,7 @@
       <c r="A164" s="19">
         <v>16</v>
       </c>
-      <c r="B164" s="112" t="s">
+      <c r="B164" s="143" t="s">
         <v>5</v>
       </c>
       <c r="C164" s="21" t="s">
@@ -19431,7 +19428,7 @@
       <c r="A165" s="19">
         <v>17</v>
       </c>
-      <c r="B165" s="113"/>
+      <c r="B165" s="145"/>
       <c r="C165" s="56" t="s">
         <v>212</v>
       </c>
@@ -19453,7 +19450,7 @@
       <c r="A166" s="19">
         <v>18</v>
       </c>
-      <c r="B166" s="121"/>
+      <c r="B166" s="129"/>
       <c r="C166" s="56" t="s">
         <v>112</v>
       </c>
@@ -19473,7 +19470,7 @@
       <c r="A167" s="19">
         <v>19</v>
       </c>
-      <c r="B167" s="122" t="s">
+      <c r="B167" s="124" t="s">
         <v>6</v>
       </c>
       <c r="C167" s="21" t="s">
@@ -19497,7 +19494,7 @@
       <c r="A168" s="19">
         <v>20</v>
       </c>
-      <c r="B168" s="119"/>
+      <c r="B168" s="125"/>
       <c r="C168" s="21" t="s">
         <v>117</v>
       </c>
@@ -19517,7 +19514,7 @@
       <c r="A169" s="19">
         <v>21</v>
       </c>
-      <c r="B169" s="119"/>
+      <c r="B169" s="125"/>
       <c r="C169" s="21" t="s">
         <v>118</v>
       </c>
@@ -19537,7 +19534,7 @@
       <c r="A170" s="19">
         <v>22</v>
       </c>
-      <c r="B170" s="119"/>
+      <c r="B170" s="125"/>
       <c r="C170" s="21" t="s">
         <v>119</v>
       </c>
@@ -19557,7 +19554,7 @@
       <c r="A171" s="19">
         <v>23</v>
       </c>
-      <c r="B171" s="119"/>
+      <c r="B171" s="125"/>
       <c r="C171" s="21" t="s">
         <v>120</v>
       </c>
@@ -19577,7 +19574,7 @@
       <c r="A172" s="19">
         <v>24</v>
       </c>
-      <c r="B172" s="119"/>
+      <c r="B172" s="125"/>
       <c r="C172" s="21" t="s">
         <v>121</v>
       </c>
@@ -19597,7 +19594,7 @@
       <c r="A173" s="19">
         <v>25</v>
       </c>
-      <c r="B173" s="119"/>
+      <c r="B173" s="125"/>
       <c r="C173" s="21" t="s">
         <v>122</v>
       </c>
@@ -19617,7 +19614,7 @@
       <c r="A174" s="19">
         <v>26</v>
       </c>
-      <c r="B174" s="119"/>
+      <c r="B174" s="125"/>
       <c r="C174" s="21" t="s">
         <v>38</v>
       </c>
@@ -19637,7 +19634,7 @@
       <c r="A175" s="19">
         <v>27</v>
       </c>
-      <c r="B175" s="122" t="s">
+      <c r="B175" s="124" t="s">
         <v>7</v>
       </c>
       <c r="C175" s="21" t="s">
@@ -19661,7 +19658,7 @@
       <c r="A176" s="19">
         <v>28</v>
       </c>
-      <c r="B176" s="119"/>
+      <c r="B176" s="125"/>
       <c r="C176" s="56" t="s">
         <v>124</v>
       </c>
@@ -19683,7 +19680,7 @@
       <c r="A177" s="19">
         <v>29</v>
       </c>
-      <c r="B177" s="119"/>
+      <c r="B177" s="125"/>
       <c r="C177" s="56" t="s">
         <v>237</v>
       </c>
@@ -19705,7 +19702,7 @@
       <c r="A178" s="19">
         <v>30</v>
       </c>
-      <c r="B178" s="119"/>
+      <c r="B178" s="125"/>
       <c r="C178" s="56" t="s">
         <v>127</v>
       </c>
@@ -19727,7 +19724,7 @@
       <c r="A179" s="19">
         <v>31</v>
       </c>
-      <c r="B179" s="119"/>
+      <c r="B179" s="125"/>
       <c r="C179" s="56" t="s">
         <v>234</v>
       </c>
@@ -19749,7 +19746,7 @@
       <c r="A180" s="19">
         <v>32</v>
       </c>
-      <c r="B180" s="119"/>
+      <c r="B180" s="125"/>
       <c r="C180" s="56" t="s">
         <v>235</v>
       </c>
@@ -19771,7 +19768,7 @@
       <c r="A181" s="19">
         <v>33</v>
       </c>
-      <c r="B181" s="112" t="s">
+      <c r="B181" s="143" t="s">
         <v>8</v>
       </c>
       <c r="C181" s="21" t="s">
@@ -19797,7 +19794,7 @@
       <c r="A182" s="22">
         <v>34</v>
       </c>
-      <c r="B182" s="113"/>
+      <c r="B182" s="145"/>
       <c r="C182" s="20" t="s">
         <v>131</v>
       </c>
@@ -19821,7 +19818,7 @@
       <c r="A183" s="22">
         <v>35</v>
       </c>
-      <c r="B183" s="114"/>
+      <c r="B183" s="144"/>
       <c r="C183" s="58" t="s">
         <v>240</v>
       </c>
@@ -19845,7 +19842,7 @@
       <c r="A184" s="16">
         <v>36</v>
       </c>
-      <c r="B184" s="115" t="s">
+      <c r="B184" s="146" t="s">
         <v>64</v>
       </c>
       <c r="C184" s="57" t="s">
@@ -19869,7 +19866,7 @@
       <c r="A185" s="19">
         <v>37</v>
       </c>
-      <c r="B185" s="116"/>
+      <c r="B185" s="147"/>
       <c r="C185" s="56" t="s">
         <v>136</v>
       </c>
@@ -19891,7 +19888,7 @@
       <c r="A186" s="19">
         <v>38</v>
       </c>
-      <c r="B186" s="117"/>
+      <c r="B186" s="148"/>
       <c r="C186" s="58" t="s">
         <v>139</v>
       </c>
@@ -19913,7 +19910,7 @@
       <c r="A187" s="19">
         <v>39</v>
       </c>
-      <c r="B187" s="117"/>
+      <c r="B187" s="148"/>
       <c r="C187" s="58" t="s">
         <v>140</v>
       </c>
@@ -19935,7 +19932,7 @@
       <c r="A188" s="19">
         <v>40</v>
       </c>
-      <c r="B188" s="117"/>
+      <c r="B188" s="148"/>
       <c r="C188" s="58" t="s">
         <v>143</v>
       </c>
@@ -19955,7 +19952,7 @@
       <c r="A189" s="19">
         <v>41</v>
       </c>
-      <c r="B189" s="117"/>
+      <c r="B189" s="148"/>
       <c r="C189" s="58" t="s">
         <v>219</v>
       </c>
@@ -19977,7 +19974,7 @@
       <c r="A190" s="24">
         <v>42</v>
       </c>
-      <c r="B190" s="118"/>
+      <c r="B190" s="133"/>
       <c r="C190" s="25" t="s">
         <v>223</v>
       </c>
@@ -20028,11 +20025,11 @@
       <c r="B204" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="C204" s="146" t="s">
+      <c r="C204" s="115" t="s">
         <v>151</v>
       </c>
-      <c r="D204" s="146"/>
-      <c r="E204" s="146"/>
+      <c r="D204" s="115"/>
+      <c r="E204" s="115"/>
       <c r="F204" s="27" t="s">
         <v>152</v>
       </c>
@@ -20041,17 +20038,17 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="128" t="s">
+      <c r="A205" s="141" t="s">
         <v>154</v>
       </c>
-      <c r="B205" s="119" t="s">
+      <c r="B205" s="125" t="s">
         <v>155</v>
       </c>
-      <c r="C205" s="147" t="s">
+      <c r="C205" s="116" t="s">
         <v>156</v>
       </c>
-      <c r="D205" s="148"/>
-      <c r="E205" s="148"/>
+      <c r="D205" s="117"/>
+      <c r="E205" s="117"/>
       <c r="F205" s="21" t="s">
         <v>157</v>
       </c>
@@ -20060,13 +20057,13 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="128"/>
-      <c r="B206" s="120"/>
-      <c r="C206" s="138" t="s">
+      <c r="A206" s="141"/>
+      <c r="B206" s="149"/>
+      <c r="C206" s="118" t="s">
         <v>156</v>
       </c>
-      <c r="D206" s="149"/>
-      <c r="E206" s="149"/>
+      <c r="D206" s="119"/>
+      <c r="E206" s="119"/>
       <c r="F206" s="20" t="s">
         <v>159</v>
       </c>
@@ -20075,15 +20072,15 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="128"/>
-      <c r="B207" s="119" t="s">
+      <c r="A207" s="141"/>
+      <c r="B207" s="125" t="s">
         <v>160</v>
       </c>
-      <c r="C207" s="142" t="s">
+      <c r="C207" s="120" t="s">
         <v>161</v>
       </c>
-      <c r="D207" s="142"/>
-      <c r="E207" s="142"/>
+      <c r="D207" s="120"/>
+      <c r="E207" s="120"/>
       <c r="F207" s="21" t="s">
         <v>157</v>
       </c>
@@ -20092,13 +20089,13 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="128"/>
-      <c r="B208" s="119"/>
-      <c r="C208" s="138" t="s">
+      <c r="A208" s="141"/>
+      <c r="B208" s="125"/>
+      <c r="C208" s="118" t="s">
         <v>161</v>
       </c>
-      <c r="D208" s="138"/>
-      <c r="E208" s="138"/>
+      <c r="D208" s="118"/>
+      <c r="E208" s="118"/>
       <c r="F208" s="21" t="s">
         <v>159</v>
       </c>
@@ -20107,15 +20104,15 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="128"/>
-      <c r="B209" s="120" t="s">
+      <c r="A209" s="141"/>
+      <c r="B209" s="149" t="s">
         <v>162</v>
       </c>
-      <c r="C209" s="139" t="s">
+      <c r="C209" s="121" t="s">
         <v>156</v>
       </c>
-      <c r="D209" s="140"/>
-      <c r="E209" s="141"/>
+      <c r="D209" s="122"/>
+      <c r="E209" s="123"/>
       <c r="F209" s="21" t="s">
         <v>157</v>
       </c>
@@ -20124,13 +20121,13 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="128"/>
-      <c r="B210" s="121"/>
-      <c r="C210" s="139" t="s">
+      <c r="A210" s="141"/>
+      <c r="B210" s="129"/>
+      <c r="C210" s="121" t="s">
         <v>156</v>
       </c>
-      <c r="D210" s="140"/>
-      <c r="E210" s="141"/>
+      <c r="D210" s="122"/>
+      <c r="E210" s="123"/>
       <c r="F210" s="21" t="s">
         <v>159</v>
       </c>
@@ -20139,15 +20136,15 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="128"/>
-      <c r="B211" s="119" t="s">
+      <c r="A211" s="141"/>
+      <c r="B211" s="125" t="s">
         <v>163</v>
       </c>
-      <c r="C211" s="142" t="s">
+      <c r="C211" s="120" t="s">
         <v>164</v>
       </c>
-      <c r="D211" s="142"/>
-      <c r="E211" s="142"/>
+      <c r="D211" s="120"/>
+      <c r="E211" s="120"/>
       <c r="F211" s="21" t="s">
         <v>157</v>
       </c>
@@ -20156,13 +20153,13 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="128"/>
-      <c r="B212" s="119"/>
-      <c r="C212" s="142" t="s">
+      <c r="A212" s="141"/>
+      <c r="B212" s="125"/>
+      <c r="C212" s="120" t="s">
         <v>164</v>
       </c>
-      <c r="D212" s="142"/>
-      <c r="E212" s="142"/>
+      <c r="D212" s="120"/>
+      <c r="E212" s="120"/>
       <c r="F212" s="21" t="s">
         <v>159</v>
       </c>
@@ -20171,17 +20168,17 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="128" t="s">
+      <c r="A213" s="141" t="s">
         <v>165</v>
       </c>
-      <c r="B213" s="119" t="s">
+      <c r="B213" s="125" t="s">
         <v>166</v>
       </c>
-      <c r="C213" s="122" t="s">
+      <c r="C213" s="124" t="s">
         <v>167</v>
       </c>
-      <c r="D213" s="119"/>
-      <c r="E213" s="119"/>
+      <c r="D213" s="125"/>
+      <c r="E213" s="125"/>
       <c r="F213" s="21" t="s">
         <v>157</v>
       </c>
@@ -20190,13 +20187,13 @@
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="128"/>
-      <c r="B214" s="119"/>
-      <c r="C214" s="119" t="s">
+      <c r="A214" s="141"/>
+      <c r="B214" s="125"/>
+      <c r="C214" s="125" t="s">
         <v>168</v>
       </c>
-      <c r="D214" s="119"/>
-      <c r="E214" s="119"/>
+      <c r="D214" s="125"/>
+      <c r="E214" s="125"/>
       <c r="F214" s="21" t="s">
         <v>159</v>
       </c>
@@ -20205,15 +20202,15 @@
       </c>
     </row>
     <row r="215" spans="1:7">
-      <c r="A215" s="128"/>
-      <c r="B215" s="119" t="s">
+      <c r="A215" s="141"/>
+      <c r="B215" s="125" t="s">
         <v>170</v>
       </c>
-      <c r="C215" s="119" t="s">
+      <c r="C215" s="125" t="s">
         <v>171</v>
       </c>
-      <c r="D215" s="119"/>
-      <c r="E215" s="119"/>
+      <c r="D215" s="125"/>
+      <c r="E215" s="125"/>
       <c r="F215" s="21" t="s">
         <v>157</v>
       </c>
@@ -20222,13 +20219,13 @@
       </c>
     </row>
     <row r="216" spans="1:7">
-      <c r="A216" s="128"/>
-      <c r="B216" s="119"/>
-      <c r="C216" s="119" t="s">
+      <c r="A216" s="141"/>
+      <c r="B216" s="125"/>
+      <c r="C216" s="125" t="s">
         <v>172</v>
       </c>
-      <c r="D216" s="119"/>
-      <c r="E216" s="119"/>
+      <c r="D216" s="125"/>
+      <c r="E216" s="125"/>
       <c r="F216" s="21" t="s">
         <v>159</v>
       </c>
@@ -20237,17 +20234,17 @@
       </c>
     </row>
     <row r="217" spans="1:7">
-      <c r="A217" s="128" t="s">
+      <c r="A217" s="141" t="s">
         <v>173</v>
       </c>
-      <c r="B217" s="119" t="s">
+      <c r="B217" s="125" t="s">
         <v>174</v>
       </c>
-      <c r="C217" s="122" t="s">
+      <c r="C217" s="124" t="s">
         <v>175</v>
       </c>
-      <c r="D217" s="119"/>
-      <c r="E217" s="119"/>
+      <c r="D217" s="125"/>
+      <c r="E217" s="125"/>
       <c r="F217" s="21" t="s">
         <v>157</v>
       </c>
@@ -20256,13 +20253,13 @@
       </c>
     </row>
     <row r="218" spans="1:7">
-      <c r="A218" s="128"/>
-      <c r="B218" s="119"/>
-      <c r="C218" s="119" t="s">
+      <c r="A218" s="141"/>
+      <c r="B218" s="125"/>
+      <c r="C218" s="125" t="s">
         <v>176</v>
       </c>
-      <c r="D218" s="119"/>
-      <c r="E218" s="119"/>
+      <c r="D218" s="125"/>
+      <c r="E218" s="125"/>
       <c r="F218" s="21" t="s">
         <v>159</v>
       </c>
@@ -20271,15 +20268,15 @@
       </c>
     </row>
     <row r="219" spans="1:7">
-      <c r="A219" s="128"/>
-      <c r="B219" s="119" t="s">
+      <c r="A219" s="141"/>
+      <c r="B219" s="125" t="s">
         <v>177</v>
       </c>
-      <c r="C219" s="122" t="s">
+      <c r="C219" s="124" t="s">
         <v>178</v>
       </c>
-      <c r="D219" s="119"/>
-      <c r="E219" s="119"/>
+      <c r="D219" s="125"/>
+      <c r="E219" s="125"/>
       <c r="F219" s="21" t="s">
         <v>157</v>
       </c>
@@ -20288,13 +20285,13 @@
       </c>
     </row>
     <row r="220" spans="1:7">
-      <c r="A220" s="129"/>
-      <c r="B220" s="130"/>
-      <c r="C220" s="130" t="s">
+      <c r="A220" s="142"/>
+      <c r="B220" s="126"/>
+      <c r="C220" s="126" t="s">
         <v>179</v>
       </c>
-      <c r="D220" s="130"/>
-      <c r="E220" s="130"/>
+      <c r="D220" s="126"/>
+      <c r="E220" s="126"/>
       <c r="F220" s="25" t="s">
         <v>159</v>
       </c>
@@ -20316,12 +20313,12 @@
       <c r="A225" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="B225" s="136" t="s">
+      <c r="B225" s="127" t="s">
         <v>183</v>
       </c>
-      <c r="C225" s="136"/>
-      <c r="D225" s="136"/>
-      <c r="E225" s="136"/>
+      <c r="C225" s="127"/>
+      <c r="D225" s="127"/>
+      <c r="E225" s="127"/>
       <c r="F225" s="33" t="s">
         <v>184</v>
       </c>
@@ -20333,12 +20330,12 @@
       <c r="A226" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="B226" s="137" t="s">
+      <c r="B226" s="128" t="s">
         <v>187</v>
       </c>
-      <c r="C226" s="121"/>
-      <c r="D226" s="121"/>
-      <c r="E226" s="121"/>
+      <c r="C226" s="129"/>
+      <c r="D226" s="129"/>
+      <c r="E226" s="129"/>
       <c r="F226" s="36" t="s">
         <v>62</v>
       </c>
@@ -20350,12 +20347,12 @@
       <c r="A227" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B227" s="132" t="s">
+      <c r="B227" s="130" t="s">
         <v>189</v>
       </c>
-      <c r="C227" s="133"/>
-      <c r="D227" s="133"/>
-      <c r="E227" s="134"/>
+      <c r="C227" s="131"/>
+      <c r="D227" s="131"/>
+      <c r="E227" s="132"/>
       <c r="F227" s="9" t="s">
         <v>158</v>
       </c>
@@ -20367,12 +20364,12 @@
       <c r="A228" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B228" s="132" t="s">
+      <c r="B228" s="130" t="s">
         <v>191</v>
       </c>
-      <c r="C228" s="133"/>
-      <c r="D228" s="133"/>
-      <c r="E228" s="134"/>
+      <c r="C228" s="131"/>
+      <c r="D228" s="131"/>
+      <c r="E228" s="132"/>
       <c r="F228" s="13" t="s">
         <v>158</v>
       </c>
@@ -20384,12 +20381,12 @@
       <c r="A229" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="B229" s="118" t="s">
+      <c r="B229" s="133" t="s">
         <v>193</v>
       </c>
-      <c r="C229" s="130"/>
-      <c r="D229" s="130"/>
-      <c r="E229" s="130"/>
+      <c r="C229" s="126"/>
+      <c r="D229" s="126"/>
+      <c r="E229" s="126"/>
       <c r="F229" s="15" t="s">
         <v>158</v>
       </c>
@@ -20434,11 +20431,11 @@
       <c r="C234" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="D234" s="135" t="s">
+      <c r="D234" s="134" t="s">
         <v>199</v>
       </c>
-      <c r="E234" s="135"/>
-      <c r="F234" s="135"/>
+      <c r="E234" s="134"/>
+      <c r="F234" s="134"/>
       <c r="G234" s="18"/>
     </row>
     <row r="235" spans="1:7">
@@ -20451,11 +20448,11 @@
       <c r="C235" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D235" s="131" t="s">
+      <c r="D235" s="135" t="s">
         <v>200</v>
       </c>
-      <c r="E235" s="131"/>
-      <c r="F235" s="131"/>
+      <c r="E235" s="135"/>
+      <c r="F235" s="135"/>
       <c r="G235" s="29"/>
     </row>
     <row r="236" spans="1:7">
@@ -20468,11 +20465,11 @@
       <c r="C236" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D236" s="131" t="s">
+      <c r="D236" s="135" t="s">
         <v>201</v>
       </c>
-      <c r="E236" s="131"/>
-      <c r="F236" s="131"/>
+      <c r="E236" s="135"/>
+      <c r="F236" s="135"/>
       <c r="G236" s="29"/>
     </row>
     <row r="237" spans="1:7">
@@ -20485,11 +20482,11 @@
       <c r="C237" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D237" s="131" t="s">
+      <c r="D237" s="135" t="s">
         <v>202</v>
       </c>
-      <c r="E237" s="131"/>
-      <c r="F237" s="131"/>
+      <c r="E237" s="135"/>
+      <c r="F237" s="135"/>
       <c r="G237" s="29"/>
     </row>
     <row r="238" spans="1:7">
@@ -20502,11 +20499,11 @@
       <c r="C238" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D238" s="131" t="s">
+      <c r="D238" s="135" t="s">
         <v>203</v>
       </c>
-      <c r="E238" s="131"/>
-      <c r="F238" s="131"/>
+      <c r="E238" s="135"/>
+      <c r="F238" s="135"/>
       <c r="G238" s="29"/>
     </row>
     <row r="239" spans="1:7">
@@ -20519,11 +20516,11 @@
       <c r="C239" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D239" s="131" t="s">
+      <c r="D239" s="135" t="s">
         <v>204</v>
       </c>
-      <c r="E239" s="131"/>
-      <c r="F239" s="131"/>
+      <c r="E239" s="135"/>
+      <c r="F239" s="135"/>
       <c r="G239" s="29"/>
     </row>
     <row r="240" spans="1:7">
@@ -20536,11 +20533,11 @@
       <c r="C240" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="D240" s="123" t="s">
+      <c r="D240" s="136" t="s">
         <v>205</v>
       </c>
-      <c r="E240" s="124"/>
-      <c r="F240" s="125"/>
+      <c r="E240" s="137"/>
+      <c r="F240" s="138"/>
       <c r="G240" s="30"/>
     </row>
     <row r="241" spans="1:7">
@@ -20553,11 +20550,11 @@
       <c r="C241" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="D241" s="123" t="s">
+      <c r="D241" s="136" t="s">
         <v>206</v>
       </c>
-      <c r="E241" s="124"/>
-      <c r="F241" s="125"/>
+      <c r="E241" s="137"/>
+      <c r="F241" s="138"/>
       <c r="G241" s="30"/>
     </row>
     <row r="242" spans="1:7">
@@ -20570,11 +20567,11 @@
       <c r="C242" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="D242" s="123" t="s">
+      <c r="D242" s="136" t="s">
         <v>207</v>
       </c>
-      <c r="E242" s="124"/>
-      <c r="F242" s="125"/>
+      <c r="E242" s="137"/>
+      <c r="F242" s="138"/>
       <c r="G242" s="30"/>
     </row>
     <row r="243" spans="1:7">
@@ -20723,51 +20720,36 @@
       <c r="C251" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="D251" s="126" t="s">
+      <c r="D251" s="139" t="s">
         <v>245</v>
       </c>
-      <c r="E251" s="127"/>
-      <c r="F251" s="127"/>
+      <c r="E251" s="140"/>
+      <c r="F251" s="140"/>
       <c r="G251" s="31"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Y3CbQBUOESlDRywGeoG/3StrDbFnCkeqkNskZfEB2tOROsi5KmkcJgzaGARx/t71p+8XW8S30YXLCnas8V4vyw==" saltValue="Hjy+0Aja5MmvK1SBdUhEOA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}" scale="115">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}" scale="115">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="C205:E205"/>
-    <mergeCell ref="C206:E206"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="C216:E216"/>
-    <mergeCell ref="C217:E217"/>
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="C219:E219"/>
-    <mergeCell ref="C220:E220"/>
-    <mergeCell ref="B225:E225"/>
-    <mergeCell ref="B226:E226"/>
-    <mergeCell ref="B227:E227"/>
-    <mergeCell ref="B228:E228"/>
-    <mergeCell ref="B229:E229"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="B181:B183"/>
+    <mergeCell ref="B184:B190"/>
+    <mergeCell ref="B205:B206"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="B149:B161"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="B164:B166"/>
+    <mergeCell ref="B167:B174"/>
+    <mergeCell ref="B175:B180"/>
     <mergeCell ref="D241:F241"/>
     <mergeCell ref="D242:F242"/>
     <mergeCell ref="D251:F251"/>
@@ -20784,16 +20766,31 @@
     <mergeCell ref="D238:F238"/>
     <mergeCell ref="D239:F239"/>
     <mergeCell ref="D240:F240"/>
-    <mergeCell ref="B149:B161"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="B164:B166"/>
-    <mergeCell ref="B167:B174"/>
-    <mergeCell ref="B175:B180"/>
-    <mergeCell ref="B181:B183"/>
-    <mergeCell ref="B184:B190"/>
-    <mergeCell ref="B205:B206"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="B209:B210"/>
+    <mergeCell ref="B227:E227"/>
+    <mergeCell ref="B228:E228"/>
+    <mergeCell ref="B229:E229"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C219:E219"/>
+    <mergeCell ref="C220:E220"/>
+    <mergeCell ref="B225:E225"/>
+    <mergeCell ref="B226:E226"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="C216:E216"/>
+    <mergeCell ref="C217:E217"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C204:E204"/>
+    <mergeCell ref="C205:E205"/>
+    <mergeCell ref="C206:E206"/>
+    <mergeCell ref="C207:E207"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -23638,19 +23635,19 @@
   </sheetData>
   <autoFilter ref="B1:J97" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
       <selection activeCell="D24" sqref="D24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>

<commit_message>
i492--avant eit2 suite update
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_EIT_suites/radiant/silicon_12_Avant_GX.xlsx
+++ b/tmp_client/doc/TMP_EIT_suites/radiant/silicon_12_Avant_GX.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\repository\tmp_client\doc\TMP_EIT_suites\radiant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD89189A-F219-4E2A-A43D-70FEBB1F8D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C9526F-325E-4C5C-A12D-7CD5309F0029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,16 +34,16 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <customWorkbookViews>
+    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2" showComments="commIndAndComment"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
     <customWorkbookView name="Jeffrey Ye - Personal View" guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2" showComments="commIndAndComment"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4193" uniqueCount="1330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4194" uniqueCount="1330">
   <si>
     <t>[suite_info]</t>
   </si>
@@ -5080,67 +5080,38 @@
     <xf numFmtId="49" fontId="9" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="5" applyBorder="1">
       <alignment vertical="center"/>
@@ -5163,26 +5134,55 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="21">
@@ -8063,7 +8063,7 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8336,8 +8336,13 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
-      <selection activeCell="G17" sqref="G17"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+      <selection activeCell="B13" sqref="B13"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -8346,13 +8351,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="B4" sqref="B4"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
-      <selection activeCell="B13" sqref="B13"/>
+    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
+      <selection activeCell="G17" sqref="G17"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -8370,7 +8370,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C42" sqref="C42"/>
+      <selection pane="bottomRight" activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -10631,10 +10631,10 @@
   <dimension ref="A1:AF194"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B173" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C196" sqref="C196"/>
+      <selection pane="bottomRight" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -13285,6 +13285,9 @@
       </c>
       <c r="E68" s="53" t="s">
         <v>927</v>
+      </c>
+      <c r="P68" s="53" t="s">
+        <v>554</v>
       </c>
       <c r="T68" s="53" t="s">
         <v>386</v>
@@ -18120,17 +18123,17 @@
       <c r="E111" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F111" s="112" t="s">
+      <c r="F111" s="143" t="s">
         <v>48</v>
       </c>
-      <c r="G111" s="113"/>
-      <c r="H111" s="113"/>
-      <c r="I111" s="113"/>
-      <c r="J111" s="113"/>
-      <c r="K111" s="113"/>
-      <c r="L111" s="113"/>
-      <c r="M111" s="113"/>
-      <c r="N111" s="114"/>
+      <c r="G111" s="144"/>
+      <c r="H111" s="144"/>
+      <c r="I111" s="144"/>
+      <c r="J111" s="144"/>
+      <c r="K111" s="144"/>
+      <c r="L111" s="144"/>
+      <c r="M111" s="144"/>
+      <c r="N111" s="145"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -19050,7 +19053,7 @@
       <c r="A149" s="19">
         <v>1</v>
       </c>
-      <c r="B149" s="143" t="s">
+      <c r="B149" s="112" t="s">
         <v>3</v>
       </c>
       <c r="C149" s="56" t="s">
@@ -19076,7 +19079,7 @@
       <c r="A150" s="19">
         <v>2</v>
       </c>
-      <c r="B150" s="144"/>
+      <c r="B150" s="114"/>
       <c r="C150" s="21" t="s">
         <v>81</v>
       </c>
@@ -19098,7 +19101,7 @@
       <c r="A151" s="19">
         <v>3</v>
       </c>
-      <c r="B151" s="144"/>
+      <c r="B151" s="114"/>
       <c r="C151" s="21" t="s">
         <v>16</v>
       </c>
@@ -19118,7 +19121,7 @@
       <c r="A152" s="19">
         <v>4</v>
       </c>
-      <c r="B152" s="144"/>
+      <c r="B152" s="114"/>
       <c r="C152" s="21" t="s">
         <v>83</v>
       </c>
@@ -19142,7 +19145,7 @@
       <c r="A153" s="19">
         <v>5</v>
       </c>
-      <c r="B153" s="144"/>
+      <c r="B153" s="114"/>
       <c r="C153" s="56" t="s">
         <v>85</v>
       </c>
@@ -19166,7 +19169,7 @@
       <c r="A154" s="19">
         <v>6</v>
       </c>
-      <c r="B154" s="144"/>
+      <c r="B154" s="114"/>
       <c r="C154" s="56" t="s">
         <v>89</v>
       </c>
@@ -19190,7 +19193,7 @@
       <c r="A155" s="19">
         <v>7</v>
       </c>
-      <c r="B155" s="144"/>
+      <c r="B155" s="114"/>
       <c r="C155" s="21" t="s">
         <v>91</v>
       </c>
@@ -19212,7 +19215,7 @@
       <c r="A156" s="19">
         <v>8</v>
       </c>
-      <c r="B156" s="144"/>
+      <c r="B156" s="114"/>
       <c r="C156" s="56" t="s">
         <v>92</v>
       </c>
@@ -19236,7 +19239,7 @@
       <c r="A157" s="19">
         <v>9</v>
       </c>
-      <c r="B157" s="144"/>
+      <c r="B157" s="114"/>
       <c r="C157" s="56" t="s">
         <v>93</v>
       </c>
@@ -19260,7 +19263,7 @@
       <c r="A158" s="19">
         <v>10</v>
       </c>
-      <c r="B158" s="144"/>
+      <c r="B158" s="114"/>
       <c r="C158" s="21" t="s">
         <v>94</v>
       </c>
@@ -19284,7 +19287,7 @@
       <c r="A159" s="19">
         <v>11</v>
       </c>
-      <c r="B159" s="144"/>
+      <c r="B159" s="114"/>
       <c r="C159" s="21" t="s">
         <v>95</v>
       </c>
@@ -19308,7 +19311,7 @@
       <c r="A160" s="19">
         <v>12</v>
       </c>
-      <c r="B160" s="144"/>
+      <c r="B160" s="114"/>
       <c r="C160" s="21" t="s">
         <v>97</v>
       </c>
@@ -19330,7 +19333,7 @@
       <c r="A161" s="19">
         <v>13</v>
       </c>
-      <c r="B161" s="129"/>
+      <c r="B161" s="121"/>
       <c r="C161" s="21" t="s">
         <v>101</v>
       </c>
@@ -19354,7 +19357,7 @@
       <c r="A162" s="19">
         <v>14</v>
       </c>
-      <c r="B162" s="124" t="s">
+      <c r="B162" s="122" t="s">
         <v>4</v>
       </c>
       <c r="C162" s="21" t="s">
@@ -19380,7 +19383,7 @@
       <c r="A163" s="19">
         <v>15</v>
       </c>
-      <c r="B163" s="125"/>
+      <c r="B163" s="119"/>
       <c r="C163" s="21" t="s">
         <v>108</v>
       </c>
@@ -19404,7 +19407,7 @@
       <c r="A164" s="19">
         <v>16</v>
       </c>
-      <c r="B164" s="143" t="s">
+      <c r="B164" s="112" t="s">
         <v>5</v>
       </c>
       <c r="C164" s="21" t="s">
@@ -19428,7 +19431,7 @@
       <c r="A165" s="19">
         <v>17</v>
       </c>
-      <c r="B165" s="145"/>
+      <c r="B165" s="113"/>
       <c r="C165" s="56" t="s">
         <v>212</v>
       </c>
@@ -19450,7 +19453,7 @@
       <c r="A166" s="19">
         <v>18</v>
       </c>
-      <c r="B166" s="129"/>
+      <c r="B166" s="121"/>
       <c r="C166" s="56" t="s">
         <v>112</v>
       </c>
@@ -19470,7 +19473,7 @@
       <c r="A167" s="19">
         <v>19</v>
       </c>
-      <c r="B167" s="124" t="s">
+      <c r="B167" s="122" t="s">
         <v>6</v>
       </c>
       <c r="C167" s="21" t="s">
@@ -19494,7 +19497,7 @@
       <c r="A168" s="19">
         <v>20</v>
       </c>
-      <c r="B168" s="125"/>
+      <c r="B168" s="119"/>
       <c r="C168" s="21" t="s">
         <v>117</v>
       </c>
@@ -19514,7 +19517,7 @@
       <c r="A169" s="19">
         <v>21</v>
       </c>
-      <c r="B169" s="125"/>
+      <c r="B169" s="119"/>
       <c r="C169" s="21" t="s">
         <v>118</v>
       </c>
@@ -19534,7 +19537,7 @@
       <c r="A170" s="19">
         <v>22</v>
       </c>
-      <c r="B170" s="125"/>
+      <c r="B170" s="119"/>
       <c r="C170" s="21" t="s">
         <v>119</v>
       </c>
@@ -19554,7 +19557,7 @@
       <c r="A171" s="19">
         <v>23</v>
       </c>
-      <c r="B171" s="125"/>
+      <c r="B171" s="119"/>
       <c r="C171" s="21" t="s">
         <v>120</v>
       </c>
@@ -19574,7 +19577,7 @@
       <c r="A172" s="19">
         <v>24</v>
       </c>
-      <c r="B172" s="125"/>
+      <c r="B172" s="119"/>
       <c r="C172" s="21" t="s">
         <v>121</v>
       </c>
@@ -19594,7 +19597,7 @@
       <c r="A173" s="19">
         <v>25</v>
       </c>
-      <c r="B173" s="125"/>
+      <c r="B173" s="119"/>
       <c r="C173" s="21" t="s">
         <v>122</v>
       </c>
@@ -19614,7 +19617,7 @@
       <c r="A174" s="19">
         <v>26</v>
       </c>
-      <c r="B174" s="125"/>
+      <c r="B174" s="119"/>
       <c r="C174" s="21" t="s">
         <v>38</v>
       </c>
@@ -19634,7 +19637,7 @@
       <c r="A175" s="19">
         <v>27</v>
       </c>
-      <c r="B175" s="124" t="s">
+      <c r="B175" s="122" t="s">
         <v>7</v>
       </c>
       <c r="C175" s="21" t="s">
@@ -19658,7 +19661,7 @@
       <c r="A176" s="19">
         <v>28</v>
       </c>
-      <c r="B176" s="125"/>
+      <c r="B176" s="119"/>
       <c r="C176" s="56" t="s">
         <v>124</v>
       </c>
@@ -19680,7 +19683,7 @@
       <c r="A177" s="19">
         <v>29</v>
       </c>
-      <c r="B177" s="125"/>
+      <c r="B177" s="119"/>
       <c r="C177" s="56" t="s">
         <v>237</v>
       </c>
@@ -19702,7 +19705,7 @@
       <c r="A178" s="19">
         <v>30</v>
       </c>
-      <c r="B178" s="125"/>
+      <c r="B178" s="119"/>
       <c r="C178" s="56" t="s">
         <v>127</v>
       </c>
@@ -19724,7 +19727,7 @@
       <c r="A179" s="19">
         <v>31</v>
       </c>
-      <c r="B179" s="125"/>
+      <c r="B179" s="119"/>
       <c r="C179" s="56" t="s">
         <v>234</v>
       </c>
@@ -19746,7 +19749,7 @@
       <c r="A180" s="19">
         <v>32</v>
       </c>
-      <c r="B180" s="125"/>
+      <c r="B180" s="119"/>
       <c r="C180" s="56" t="s">
         <v>235</v>
       </c>
@@ -19768,7 +19771,7 @@
       <c r="A181" s="19">
         <v>33</v>
       </c>
-      <c r="B181" s="143" t="s">
+      <c r="B181" s="112" t="s">
         <v>8</v>
       </c>
       <c r="C181" s="21" t="s">
@@ -19794,7 +19797,7 @@
       <c r="A182" s="22">
         <v>34</v>
       </c>
-      <c r="B182" s="145"/>
+      <c r="B182" s="113"/>
       <c r="C182" s="20" t="s">
         <v>131</v>
       </c>
@@ -19818,7 +19821,7 @@
       <c r="A183" s="22">
         <v>35</v>
       </c>
-      <c r="B183" s="144"/>
+      <c r="B183" s="114"/>
       <c r="C183" s="58" t="s">
         <v>240</v>
       </c>
@@ -19842,7 +19845,7 @@
       <c r="A184" s="16">
         <v>36</v>
       </c>
-      <c r="B184" s="146" t="s">
+      <c r="B184" s="115" t="s">
         <v>64</v>
       </c>
       <c r="C184" s="57" t="s">
@@ -19866,7 +19869,7 @@
       <c r="A185" s="19">
         <v>37</v>
       </c>
-      <c r="B185" s="147"/>
+      <c r="B185" s="116"/>
       <c r="C185" s="56" t="s">
         <v>136</v>
       </c>
@@ -19888,7 +19891,7 @@
       <c r="A186" s="19">
         <v>38</v>
       </c>
-      <c r="B186" s="148"/>
+      <c r="B186" s="117"/>
       <c r="C186" s="58" t="s">
         <v>139</v>
       </c>
@@ -19910,7 +19913,7 @@
       <c r="A187" s="19">
         <v>39</v>
       </c>
-      <c r="B187" s="148"/>
+      <c r="B187" s="117"/>
       <c r="C187" s="58" t="s">
         <v>140</v>
       </c>
@@ -19932,7 +19935,7 @@
       <c r="A188" s="19">
         <v>40</v>
       </c>
-      <c r="B188" s="148"/>
+      <c r="B188" s="117"/>
       <c r="C188" s="58" t="s">
         <v>143</v>
       </c>
@@ -19952,7 +19955,7 @@
       <c r="A189" s="19">
         <v>41</v>
       </c>
-      <c r="B189" s="148"/>
+      <c r="B189" s="117"/>
       <c r="C189" s="58" t="s">
         <v>219</v>
       </c>
@@ -19974,7 +19977,7 @@
       <c r="A190" s="24">
         <v>42</v>
       </c>
-      <c r="B190" s="133"/>
+      <c r="B190" s="118"/>
       <c r="C190" s="25" t="s">
         <v>223</v>
       </c>
@@ -20025,11 +20028,11 @@
       <c r="B204" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="C204" s="115" t="s">
+      <c r="C204" s="146" t="s">
         <v>151</v>
       </c>
-      <c r="D204" s="115"/>
-      <c r="E204" s="115"/>
+      <c r="D204" s="146"/>
+      <c r="E204" s="146"/>
       <c r="F204" s="27" t="s">
         <v>152</v>
       </c>
@@ -20038,17 +20041,17 @@
       </c>
     </row>
     <row r="205" spans="1:7">
-      <c r="A205" s="141" t="s">
+      <c r="A205" s="128" t="s">
         <v>154</v>
       </c>
-      <c r="B205" s="125" t="s">
+      <c r="B205" s="119" t="s">
         <v>155</v>
       </c>
-      <c r="C205" s="116" t="s">
+      <c r="C205" s="147" t="s">
         <v>156</v>
       </c>
-      <c r="D205" s="117"/>
-      <c r="E205" s="117"/>
+      <c r="D205" s="148"/>
+      <c r="E205" s="148"/>
       <c r="F205" s="21" t="s">
         <v>157</v>
       </c>
@@ -20057,13 +20060,13 @@
       </c>
     </row>
     <row r="206" spans="1:7">
-      <c r="A206" s="141"/>
-      <c r="B206" s="149"/>
-      <c r="C206" s="118" t="s">
+      <c r="A206" s="128"/>
+      <c r="B206" s="120"/>
+      <c r="C206" s="138" t="s">
         <v>156</v>
       </c>
-      <c r="D206" s="119"/>
-      <c r="E206" s="119"/>
+      <c r="D206" s="149"/>
+      <c r="E206" s="149"/>
       <c r="F206" s="20" t="s">
         <v>159</v>
       </c>
@@ -20072,15 +20075,15 @@
       </c>
     </row>
     <row r="207" spans="1:7">
-      <c r="A207" s="141"/>
-      <c r="B207" s="125" t="s">
+      <c r="A207" s="128"/>
+      <c r="B207" s="119" t="s">
         <v>160</v>
       </c>
-      <c r="C207" s="120" t="s">
+      <c r="C207" s="142" t="s">
         <v>161</v>
       </c>
-      <c r="D207" s="120"/>
-      <c r="E207" s="120"/>
+      <c r="D207" s="142"/>
+      <c r="E207" s="142"/>
       <c r="F207" s="21" t="s">
         <v>157</v>
       </c>
@@ -20089,13 +20092,13 @@
       </c>
     </row>
     <row r="208" spans="1:7">
-      <c r="A208" s="141"/>
-      <c r="B208" s="125"/>
-      <c r="C208" s="118" t="s">
+      <c r="A208" s="128"/>
+      <c r="B208" s="119"/>
+      <c r="C208" s="138" t="s">
         <v>161</v>
       </c>
-      <c r="D208" s="118"/>
-      <c r="E208" s="118"/>
+      <c r="D208" s="138"/>
+      <c r="E208" s="138"/>
       <c r="F208" s="21" t="s">
         <v>159</v>
       </c>
@@ -20104,15 +20107,15 @@
       </c>
     </row>
     <row r="209" spans="1:7">
-      <c r="A209" s="141"/>
-      <c r="B209" s="149" t="s">
+      <c r="A209" s="128"/>
+      <c r="B209" s="120" t="s">
         <v>162</v>
       </c>
-      <c r="C209" s="121" t="s">
+      <c r="C209" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="D209" s="122"/>
-      <c r="E209" s="123"/>
+      <c r="D209" s="140"/>
+      <c r="E209" s="141"/>
       <c r="F209" s="21" t="s">
         <v>157</v>
       </c>
@@ -20121,13 +20124,13 @@
       </c>
     </row>
     <row r="210" spans="1:7">
-      <c r="A210" s="141"/>
-      <c r="B210" s="129"/>
-      <c r="C210" s="121" t="s">
+      <c r="A210" s="128"/>
+      <c r="B210" s="121"/>
+      <c r="C210" s="139" t="s">
         <v>156</v>
       </c>
-      <c r="D210" s="122"/>
-      <c r="E210" s="123"/>
+      <c r="D210" s="140"/>
+      <c r="E210" s="141"/>
       <c r="F210" s="21" t="s">
         <v>159</v>
       </c>
@@ -20136,15 +20139,15 @@
       </c>
     </row>
     <row r="211" spans="1:7">
-      <c r="A211" s="141"/>
-      <c r="B211" s="125" t="s">
+      <c r="A211" s="128"/>
+      <c r="B211" s="119" t="s">
         <v>163</v>
       </c>
-      <c r="C211" s="120" t="s">
+      <c r="C211" s="142" t="s">
         <v>164</v>
       </c>
-      <c r="D211" s="120"/>
-      <c r="E211" s="120"/>
+      <c r="D211" s="142"/>
+      <c r="E211" s="142"/>
       <c r="F211" s="21" t="s">
         <v>157</v>
       </c>
@@ -20153,13 +20156,13 @@
       </c>
     </row>
     <row r="212" spans="1:7">
-      <c r="A212" s="141"/>
-      <c r="B212" s="125"/>
-      <c r="C212" s="120" t="s">
+      <c r="A212" s="128"/>
+      <c r="B212" s="119"/>
+      <c r="C212" s="142" t="s">
         <v>164</v>
       </c>
-      <c r="D212" s="120"/>
-      <c r="E212" s="120"/>
+      <c r="D212" s="142"/>
+      <c r="E212" s="142"/>
       <c r="F212" s="21" t="s">
         <v>159</v>
       </c>
@@ -20168,17 +20171,17 @@
       </c>
     </row>
     <row r="213" spans="1:7">
-      <c r="A213" s="141" t="s">
+      <c r="A213" s="128" t="s">
         <v>165</v>
       </c>
-      <c r="B213" s="125" t="s">
+      <c r="B213" s="119" t="s">
         <v>166</v>
       </c>
-      <c r="C213" s="124" t="s">
+      <c r="C213" s="122" t="s">
         <v>167</v>
       </c>
-      <c r="D213" s="125"/>
-      <c r="E213" s="125"/>
+      <c r="D213" s="119"/>
+      <c r="E213" s="119"/>
       <c r="F213" s="21" t="s">
         <v>157</v>
       </c>
@@ -20187,13 +20190,13 @@
       </c>
     </row>
     <row r="214" spans="1:7">
-      <c r="A214" s="141"/>
-      <c r="B214" s="125"/>
-      <c r="C214" s="125" t="s">
+      <c r="A214" s="128"/>
+      <c r="B214" s="119"/>
+      <c r="C214" s="119" t="s">
         <v>168</v>
       </c>
-      <c r="D214" s="125"/>
-      <c r="E214" s="125"/>
+      <c r="D214" s="119"/>
+      <c r="E214" s="119"/>
       <c r="F214" s="21" t="s">
         <v>159</v>
       </c>
@@ -20202,15 +20205,15 @@
       </c>
     </row>
     <row r="215" spans="1:7">
-      <c r="A215" s="141"/>
-      <c r="B215" s="125" t="s">
+      <c r="A215" s="128"/>
+      <c r="B215" s="119" t="s">
         <v>170</v>
       </c>
-      <c r="C215" s="125" t="s">
+      <c r="C215" s="119" t="s">
         <v>171</v>
       </c>
-      <c r="D215" s="125"/>
-      <c r="E215" s="125"/>
+      <c r="D215" s="119"/>
+      <c r="E215" s="119"/>
       <c r="F215" s="21" t="s">
         <v>157</v>
       </c>
@@ -20219,13 +20222,13 @@
       </c>
     </row>
     <row r="216" spans="1:7">
-      <c r="A216" s="141"/>
-      <c r="B216" s="125"/>
-      <c r="C216" s="125" t="s">
+      <c r="A216" s="128"/>
+      <c r="B216" s="119"/>
+      <c r="C216" s="119" t="s">
         <v>172</v>
       </c>
-      <c r="D216" s="125"/>
-      <c r="E216" s="125"/>
+      <c r="D216" s="119"/>
+      <c r="E216" s="119"/>
       <c r="F216" s="21" t="s">
         <v>159</v>
       </c>
@@ -20234,17 +20237,17 @@
       </c>
     </row>
     <row r="217" spans="1:7">
-      <c r="A217" s="141" t="s">
+      <c r="A217" s="128" t="s">
         <v>173</v>
       </c>
-      <c r="B217" s="125" t="s">
+      <c r="B217" s="119" t="s">
         <v>174</v>
       </c>
-      <c r="C217" s="124" t="s">
+      <c r="C217" s="122" t="s">
         <v>175</v>
       </c>
-      <c r="D217" s="125"/>
-      <c r="E217" s="125"/>
+      <c r="D217" s="119"/>
+      <c r="E217" s="119"/>
       <c r="F217" s="21" t="s">
         <v>157</v>
       </c>
@@ -20253,13 +20256,13 @@
       </c>
     </row>
     <row r="218" spans="1:7">
-      <c r="A218" s="141"/>
-      <c r="B218" s="125"/>
-      <c r="C218" s="125" t="s">
+      <c r="A218" s="128"/>
+      <c r="B218" s="119"/>
+      <c r="C218" s="119" t="s">
         <v>176</v>
       </c>
-      <c r="D218" s="125"/>
-      <c r="E218" s="125"/>
+      <c r="D218" s="119"/>
+      <c r="E218" s="119"/>
       <c r="F218" s="21" t="s">
         <v>159</v>
       </c>
@@ -20268,15 +20271,15 @@
       </c>
     </row>
     <row r="219" spans="1:7">
-      <c r="A219" s="141"/>
-      <c r="B219" s="125" t="s">
+      <c r="A219" s="128"/>
+      <c r="B219" s="119" t="s">
         <v>177</v>
       </c>
-      <c r="C219" s="124" t="s">
+      <c r="C219" s="122" t="s">
         <v>178</v>
       </c>
-      <c r="D219" s="125"/>
-      <c r="E219" s="125"/>
+      <c r="D219" s="119"/>
+      <c r="E219" s="119"/>
       <c r="F219" s="21" t="s">
         <v>157</v>
       </c>
@@ -20285,13 +20288,13 @@
       </c>
     </row>
     <row r="220" spans="1:7">
-      <c r="A220" s="142"/>
-      <c r="B220" s="126"/>
-      <c r="C220" s="126" t="s">
+      <c r="A220" s="129"/>
+      <c r="B220" s="130"/>
+      <c r="C220" s="130" t="s">
         <v>179</v>
       </c>
-      <c r="D220" s="126"/>
-      <c r="E220" s="126"/>
+      <c r="D220" s="130"/>
+      <c r="E220" s="130"/>
       <c r="F220" s="25" t="s">
         <v>159</v>
       </c>
@@ -20313,12 +20316,12 @@
       <c r="A225" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="B225" s="127" t="s">
+      <c r="B225" s="136" t="s">
         <v>183</v>
       </c>
-      <c r="C225" s="127"/>
-      <c r="D225" s="127"/>
-      <c r="E225" s="127"/>
+      <c r="C225" s="136"/>
+      <c r="D225" s="136"/>
+      <c r="E225" s="136"/>
       <c r="F225" s="33" t="s">
         <v>184</v>
       </c>
@@ -20330,12 +20333,12 @@
       <c r="A226" s="35" t="s">
         <v>186</v>
       </c>
-      <c r="B226" s="128" t="s">
+      <c r="B226" s="137" t="s">
         <v>187</v>
       </c>
-      <c r="C226" s="129"/>
-      <c r="D226" s="129"/>
-      <c r="E226" s="129"/>
+      <c r="C226" s="121"/>
+      <c r="D226" s="121"/>
+      <c r="E226" s="121"/>
       <c r="F226" s="36" t="s">
         <v>62</v>
       </c>
@@ -20347,12 +20350,12 @@
       <c r="A227" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="B227" s="130" t="s">
+      <c r="B227" s="132" t="s">
         <v>189</v>
       </c>
-      <c r="C227" s="131"/>
-      <c r="D227" s="131"/>
-      <c r="E227" s="132"/>
+      <c r="C227" s="133"/>
+      <c r="D227" s="133"/>
+      <c r="E227" s="134"/>
       <c r="F227" s="9" t="s">
         <v>158</v>
       </c>
@@ -20364,12 +20367,12 @@
       <c r="A228" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="B228" s="130" t="s">
+      <c r="B228" s="132" t="s">
         <v>191</v>
       </c>
-      <c r="C228" s="131"/>
-      <c r="D228" s="131"/>
-      <c r="E228" s="132"/>
+      <c r="C228" s="133"/>
+      <c r="D228" s="133"/>
+      <c r="E228" s="134"/>
       <c r="F228" s="13" t="s">
         <v>158</v>
       </c>
@@ -20381,12 +20384,12 @@
       <c r="A229" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="B229" s="133" t="s">
+      <c r="B229" s="118" t="s">
         <v>193</v>
       </c>
-      <c r="C229" s="126"/>
-      <c r="D229" s="126"/>
-      <c r="E229" s="126"/>
+      <c r="C229" s="130"/>
+      <c r="D229" s="130"/>
+      <c r="E229" s="130"/>
       <c r="F229" s="15" t="s">
         <v>158</v>
       </c>
@@ -20431,11 +20434,11 @@
       <c r="C234" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="D234" s="134" t="s">
+      <c r="D234" s="135" t="s">
         <v>199</v>
       </c>
-      <c r="E234" s="134"/>
-      <c r="F234" s="134"/>
+      <c r="E234" s="135"/>
+      <c r="F234" s="135"/>
       <c r="G234" s="18"/>
     </row>
     <row r="235" spans="1:7">
@@ -20448,11 +20451,11 @@
       <c r="C235" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D235" s="135" t="s">
+      <c r="D235" s="131" t="s">
         <v>200</v>
       </c>
-      <c r="E235" s="135"/>
-      <c r="F235" s="135"/>
+      <c r="E235" s="131"/>
+      <c r="F235" s="131"/>
       <c r="G235" s="29"/>
     </row>
     <row r="236" spans="1:7">
@@ -20465,11 +20468,11 @@
       <c r="C236" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D236" s="135" t="s">
+      <c r="D236" s="131" t="s">
         <v>201</v>
       </c>
-      <c r="E236" s="135"/>
-      <c r="F236" s="135"/>
+      <c r="E236" s="131"/>
+      <c r="F236" s="131"/>
       <c r="G236" s="29"/>
     </row>
     <row r="237" spans="1:7">
@@ -20482,11 +20485,11 @@
       <c r="C237" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D237" s="135" t="s">
+      <c r="D237" s="131" t="s">
         <v>202</v>
       </c>
-      <c r="E237" s="135"/>
-      <c r="F237" s="135"/>
+      <c r="E237" s="131"/>
+      <c r="F237" s="131"/>
       <c r="G237" s="29"/>
     </row>
     <row r="238" spans="1:7">
@@ -20499,11 +20502,11 @@
       <c r="C238" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D238" s="135" t="s">
+      <c r="D238" s="131" t="s">
         <v>203</v>
       </c>
-      <c r="E238" s="135"/>
-      <c r="F238" s="135"/>
+      <c r="E238" s="131"/>
+      <c r="F238" s="131"/>
       <c r="G238" s="29"/>
     </row>
     <row r="239" spans="1:7">
@@ -20516,11 +20519,11 @@
       <c r="C239" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="D239" s="135" t="s">
+      <c r="D239" s="131" t="s">
         <v>204</v>
       </c>
-      <c r="E239" s="135"/>
-      <c r="F239" s="135"/>
+      <c r="E239" s="131"/>
+      <c r="F239" s="131"/>
       <c r="G239" s="29"/>
     </row>
     <row r="240" spans="1:7">
@@ -20533,11 +20536,11 @@
       <c r="C240" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="D240" s="136" t="s">
+      <c r="D240" s="123" t="s">
         <v>205</v>
       </c>
-      <c r="E240" s="137"/>
-      <c r="F240" s="138"/>
+      <c r="E240" s="124"/>
+      <c r="F240" s="125"/>
       <c r="G240" s="30"/>
     </row>
     <row r="241" spans="1:7">
@@ -20550,11 +20553,11 @@
       <c r="C241" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="D241" s="136" t="s">
+      <c r="D241" s="123" t="s">
         <v>206</v>
       </c>
-      <c r="E241" s="137"/>
-      <c r="F241" s="138"/>
+      <c r="E241" s="124"/>
+      <c r="F241" s="125"/>
       <c r="G241" s="30"/>
     </row>
     <row r="242" spans="1:7">
@@ -20567,11 +20570,11 @@
       <c r="C242" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="D242" s="136" t="s">
+      <c r="D242" s="123" t="s">
         <v>207</v>
       </c>
-      <c r="E242" s="137"/>
-      <c r="F242" s="138"/>
+      <c r="E242" s="124"/>
+      <c r="F242" s="125"/>
       <c r="G242" s="30"/>
     </row>
     <row r="243" spans="1:7">
@@ -20720,36 +20723,51 @@
       <c r="C251" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="D251" s="139" t="s">
+      <c r="D251" s="126" t="s">
         <v>245</v>
       </c>
-      <c r="E251" s="140"/>
-      <c r="F251" s="140"/>
+      <c r="E251" s="127"/>
+      <c r="F251" s="127"/>
       <c r="G251" s="31"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Y3CbQBUOESlDRywGeoG/3StrDbFnCkeqkNskZfEB2tOROsi5KmkcJgzaGARx/t71p+8XW8S30YXLCnas8V4vyw==" saltValue="Hjy+0Aja5MmvK1SBdUhEOA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
-    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}" scale="115">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115">
+    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}" scale="115">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="B181:B183"/>
-    <mergeCell ref="B184:B190"/>
-    <mergeCell ref="B205:B206"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="B209:B210"/>
-    <mergeCell ref="B149:B161"/>
-    <mergeCell ref="B162:B163"/>
-    <mergeCell ref="B164:B166"/>
-    <mergeCell ref="B167:B174"/>
-    <mergeCell ref="B175:B180"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C204:E204"/>
+    <mergeCell ref="C205:E205"/>
+    <mergeCell ref="C206:E206"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="C216:E216"/>
+    <mergeCell ref="C217:E217"/>
+    <mergeCell ref="C218:E218"/>
+    <mergeCell ref="C219:E219"/>
+    <mergeCell ref="C220:E220"/>
+    <mergeCell ref="B225:E225"/>
+    <mergeCell ref="B226:E226"/>
+    <mergeCell ref="B227:E227"/>
+    <mergeCell ref="B228:E228"/>
+    <mergeCell ref="B229:E229"/>
+    <mergeCell ref="D234:F234"/>
+    <mergeCell ref="D235:F235"/>
     <mergeCell ref="D241:F241"/>
     <mergeCell ref="D242:F242"/>
     <mergeCell ref="D251:F251"/>
@@ -20766,31 +20784,16 @@
     <mergeCell ref="D238:F238"/>
     <mergeCell ref="D239:F239"/>
     <mergeCell ref="D240:F240"/>
-    <mergeCell ref="B227:E227"/>
-    <mergeCell ref="B228:E228"/>
-    <mergeCell ref="B229:E229"/>
-    <mergeCell ref="D234:F234"/>
-    <mergeCell ref="D235:F235"/>
-    <mergeCell ref="C218:E218"/>
-    <mergeCell ref="C219:E219"/>
-    <mergeCell ref="C220:E220"/>
-    <mergeCell ref="B225:E225"/>
-    <mergeCell ref="B226:E226"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="C216:E216"/>
-    <mergeCell ref="C217:E217"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="C205:E205"/>
-    <mergeCell ref="C206:E206"/>
-    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="B149:B161"/>
+    <mergeCell ref="B162:B163"/>
+    <mergeCell ref="B164:B166"/>
+    <mergeCell ref="B167:B174"/>
+    <mergeCell ref="B175:B180"/>
+    <mergeCell ref="B181:B183"/>
+    <mergeCell ref="B184:B190"/>
+    <mergeCell ref="B205:B206"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="B209:B210"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -23635,19 +23638,19 @@
   </sheetData>
   <autoFilter ref="B1:J97" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <customSheetViews>
-    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <selection activeCell="D24" sqref="D24"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
-      <selection activeCell="E26" sqref="E26"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{AF5BD280-20CF-4CAD-BCEB-50E8F0E6BE98}">
       <selection activeCell="D24" sqref="D24"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>